<commit_message>
Update test program for using template override
</commit_message>
<xml_diff>
--- a/source_data/protocols/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/protocols/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/CDISC_Pilot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/protocols/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99387F1B-65F9-4F46-8CE0-FAAC130D17A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996C1438-F157-DE42-A612-2D509FE36AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44980" yWindow="500" windowWidth="56420" windowHeight="27240" firstSheet="9" activeTab="18" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView minimized="1" xWindow="28700" yWindow="500" windowWidth="41180" windowHeight="27240" firstSheet="14" activeTab="26" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -37,8 +37,9 @@
     <sheet name="studyDesignEncounters" sheetId="12" r:id="rId22"/>
     <sheet name="studyDesignElements" sheetId="13" r:id="rId23"/>
     <sheet name="dictionaries" sheetId="20" r:id="rId24"/>
-    <sheet name="studyDesignContent" sheetId="16" r:id="rId25"/>
-    <sheet name="configuration" sheetId="10" r:id="rId26"/>
+    <sheet name="lillyFormat" sheetId="16" r:id="rId25"/>
+    <sheet name="m11Format" sheetId="28" r:id="rId26"/>
+    <sheet name="configuration" sheetId="10" r:id="rId27"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1959" uniqueCount="877">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2286" uniqueCount="1181">
   <si>
     <t>Screening</t>
   </si>
@@ -4796,6 +4797,928 @@
   <si>
     <t>Secondary Objective</t>
   </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>PROTOCOL SUMMARY</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>Protocol Synopsis</t>
+  </si>
+  <si>
+    <t>&lt;usdm:macro id="section" name="title_page" template="m11"/&gt;</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>Primary and Secondary Objectives and Estimands</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>Overall Design</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Committees&lt;/b&gt;
+&lt;p&gt;A Data Safety Monitoring Board (DSMB), chaired by an external cardiologist, will meet after 75, 150, 225, and 300 patients have completed 1 month of treatment. The DSMB will review cardiovascular findings to decide if discontinuation of the study or any treatment arm is appropriate, if additional cardiovascular monitoring is required, if further cardiovascular monitoring is unnecessary, or if adjustment of dose within a treatment arm (or arms) is appropriate (see Section 3.9.4).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Trial Schema</t>
+  </si>
+  <si>
+    <t>&lt;usdm:macro id="image" file="study_design.png" type="png"/&gt;
+&lt;p&gt;&lt;b&gt;Figure LZZT.1. Illustration of study design for Protocol H2Q-MC-LZZT(c).&lt;/b&gt;&lt;/p&gt;
+&lt;p&gt;Following informed consent, patients will be screened at Visit 1. At screening, patients will undergo complete neuropsychiatric assessment, psychometric testing, and general medical assessment (including medical history, pre-existing conditions, physical examination). In addition, vital signs, temperature, medication history, electrocardiogram (ECG), chest x-ray, and safety laboratories will be obtained. During the screening visit, patients will wear a placebo TTS to determine willingness and ability to comply with transdermal administration procedures. If patients have not had central nervous system (CNS) imaging in the previous 12 months, a computed tomography (CT) or magnetic resonance imaging (MRI) scan will be obtained. If patients are insulin dependent diabetics, a hemoglobin A 1c will be obtained. Screening exams and procedures may be performed after Visit 1; however, their results must be completed and available prior to randomization. The screening process should occur within 2 weeks of randomization (Visit 3 of the study).&lt;/p&gt;
+&lt;p&gt;Patients who meet enrollment criteria from Visit 1 will proceed to Visit 2 at which time they will undergo a 24-hour Ambulatory ECG. At Visit 3 the Ambulatory ECG will be removed and patients will be randomized to 1 of 3 treatment arms. The treatment arms will include a placebo arm, a low-dose xanomeline arm (50 cm 2 TTS Formulation E, 54 mg xanomeline), and a high-dose xanomeline arm (75 cm 2 TTS Formulation E, 81 mg xanomeline). All patients receiving xanomeline will be started at 50 cm 2 TTS Formulation E. For the first 8 weeks of treatment, patients will be assessed at clinic visits every 2 weeks and, thereafter, at clinic visits every 4 weeks. Patients who discontinue prior to Visit 12 (Week 24) will be brought back for full efficacy assessments at or near to 24 weeks, whenever possible.&lt;/p&gt;
+&lt;p&gt;At Visits 3, 8, 10, and 12, efficacy instruments (ADAS-Cog, CIBIC+, and DAD) will be administered. NPI-X will be administered at 2-week intervals either at clinic visits or via a telephone interview. Vital signs, temperature, and an assessment of adverse events will be obtained at all clinic visits. An electrocardiogram (ECG), and chemistry/hematology safety labs will be obtained at Visits 4, 5, 7, 8, 9, 10, 11, 12, and 13. Urinalysis will be done at Visits 4, 9, and 12. Use of concomitant medications will be collected at Visits 3, 4, 5, 7, 8, 9, 10, 11, 12, and 13. Plasma levels of xanomeline and metabolites will be obtained at Visits 3, 4, 5, 7, 9, and 11. At Visits 3, 4, 5, 7, 8, 9, 10, 11, and 12, medications will be dispensed to the patients.&lt;/p&gt;
+&lt;p&gt;Visits 1 through 13 should be scheduled relative to Visit 3 (Week 0 - randomization). Visits 4, 5, 7, 8, and 13 should occur within 3 days of their scheduled date. Visits 9, 10, 11, and 12 should occur within 4 days of their scheduled date. At Visit 13 patients will be given the option to enter the open-label extension phase (see Section 3.10.3. Study Extensions).&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>Schedule of Activities</t>
+  </si>
+  <si>
+    <t>INTRODUCTION</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>Purpose of Trial</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>Summary of Benefits and Risks</t>
+  </si>
+  <si>
+    <t>2.2.1</t>
+  </si>
+  <si>
+    <t>Benefit Summary</t>
+  </si>
+  <si>
+    <t>2.2.2</t>
+  </si>
+  <si>
+    <t>Risk Summary and Mitigation Strategy</t>
+  </si>
+  <si>
+    <t>2.2.3</t>
+  </si>
+  <si>
+    <t>Overall Benefit:Risk Conclusion</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>TRIAL OBJECTIVES AND ESTIMANDS</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>Primary Objective(s) and Associated Estimand(s)</t>
+  </si>
+  <si>
+    <t>3.1.1</t>
+  </si>
+  <si>
+    <t>{Primary Estimand}</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>Secondary Objective(s) and Associated Estimand(s)</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>Exploratory Objective(s)</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>TRIAL DESIGN</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>Description of Trial Design</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Approximately 300 patients will be enrolled (see Schedule of Events for Protocol H2Q-MC-LZZT(c), Attachment LZZT.1).&lt;/p&gt;
+&lt;p&gt;&lt;strong&gt;Duration&lt;/strong&gt;&lt;/p&gt;
+&lt;p&gt;SOMETHING HERE&lt;/p&gt;
+&lt;p&gt;Patients with probable mild to moderate AD will be studied in a randomized, double-blind, parallel (3 arm), placebo-controlled trial of 26 weeks duration. The study will be conducted on an outpatient basis.&lt;/p&gt;
+&lt;p&gt;At Visit 1, patients who meet the enrollment criteria of Mini-Mental State Examination (MMSE) score of 10 to 23 (Attachment LZZT.6), Hachinski Ischemia Score ≤4 (Attachment LZZT.8), a physical exam, safety labs, ECG, and urinalysis, will proceed to Visit 2 and Visit 3. At Visit 3, patients whose CNS imaging and other pending labs from Visit 1 satisfy the inclusion criteria (Section 3.4.2.1) will be enrolled in the study. Approximately 300 patients with a diagnosis of probable mild to moderate AD will be enrolled in the study.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
+  </si>
+  <si>
+    <t>Stakeholder Input into Design</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>Rationale for Trial Design</t>
+  </si>
+  <si>
+    <t>4.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rationale for Intervention Model     </t>
+  </si>
+  <si>
+    <t>4.2.2</t>
+  </si>
+  <si>
+    <t>Rationale for Duration</t>
+  </si>
+  <si>
+    <t>4.2.3</t>
+  </si>
+  <si>
+    <t>Rationale for Estimands</t>
+  </si>
+  <si>
+    <t>4.2.4</t>
+  </si>
+  <si>
+    <t>Rationale for Interim Analysis</t>
+  </si>
+  <si>
+    <t>4.2.5</t>
+  </si>
+  <si>
+    <t>Rationale for Control Type</t>
+  </si>
+  <si>
+    <t>4.2.6</t>
+  </si>
+  <si>
+    <t>Rationale for Adaptive or Novel Trial Design</t>
+  </si>
+  <si>
+    <t>4.2.7</t>
+  </si>
+  <si>
+    <t>Rationale for Other Trial Design Aspects</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>Trial Stopping Rules</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>Start of Trial and End of Trial</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>Access to Trial Intervention After End of Trial</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>TRIAL POPULATION</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>Description of Trial Population and Rationale</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>5.4</t>
+  </si>
+  <si>
+    <t>Contraception</t>
+  </si>
+  <si>
+    <t>5.4.1</t>
+  </si>
+  <si>
+    <t>Definitions Related to Childbearing Potential</t>
+  </si>
+  <si>
+    <t>5.4.2</t>
+  </si>
+  <si>
+    <t>Contraception Requirements</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>Lifestyle Restrictions</t>
+  </si>
+  <si>
+    <t>5.5.1</t>
+  </si>
+  <si>
+    <t>Meals and Dietary Restrictions</t>
+  </si>
+  <si>
+    <t>5.5.2</t>
+  </si>
+  <si>
+    <t>Caffeine, Alcohol, Tobacco,and Other Restrictions</t>
+  </si>
+  <si>
+    <t>5.5.3</t>
+  </si>
+  <si>
+    <t>Physical Activity Restrictions</t>
+  </si>
+  <si>
+    <t>5.5.4</t>
+  </si>
+  <si>
+    <t>Other Activity Restrictions</t>
+  </si>
+  <si>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t>Screen Failure and Rescreening</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>TRIAL INTERVENTION AND CONCOMITANT THERAPY</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>Overview of Trial Interventions</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>Description of Investigational Trial Intervention</t>
+  </si>
+  <si>
+    <t>6.3</t>
+  </si>
+  <si>
+    <t>Rationale for Investigational Trial Intervention Dose and Regimen</t>
+  </si>
+  <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>Investigational Trial Intervention Administration</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>Investigational Trial Intervention Dose Modification</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>Management of Investigational Trial Intervention Overdose</t>
+  </si>
+  <si>
+    <t>6.7</t>
+  </si>
+  <si>
+    <t>Preparation,Storage,Handling and Accountability of Investigational Trial Intervention(s)</t>
+  </si>
+  <si>
+    <t>6.7.1</t>
+  </si>
+  <si>
+    <t>Preparation of Investigational Trial Intervention(s)</t>
+  </si>
+  <si>
+    <t>6.7.2</t>
+  </si>
+  <si>
+    <t>Storage and Handling of Investigational Trial Intervention</t>
+  </si>
+  <si>
+    <t>6.7.3</t>
+  </si>
+  <si>
+    <t>Accountability of Investigational Trial Intervention</t>
+  </si>
+  <si>
+    <t>6.8</t>
+  </si>
+  <si>
+    <t>Investigational Trial Intervention Assignment,Randomisation and Blinding</t>
+  </si>
+  <si>
+    <t>6.8.1</t>
+  </si>
+  <si>
+    <t>Participant Assignment to Investigational Trial Intervention</t>
+  </si>
+  <si>
+    <t>6.8.2</t>
+  </si>
+  <si>
+    <t>Randomisation</t>
+  </si>
+  <si>
+    <t>6.8.3</t>
+  </si>
+  <si>
+    <t>{Blinding}</t>
+  </si>
+  <si>
+    <t>6.8.4</t>
+  </si>
+  <si>
+    <t>{Emergency Unblinding at the Site}</t>
+  </si>
+  <si>
+    <t>6.9</t>
+  </si>
+  <si>
+    <t>Investigational Trial Intervention Compliance</t>
+  </si>
+  <si>
+    <t>6.10</t>
+  </si>
+  <si>
+    <t>Description of Non-Investigational Trial Intervention(s)</t>
+  </si>
+  <si>
+    <t>6.10.1</t>
+  </si>
+  <si>
+    <t>{Background Intervention}</t>
+  </si>
+  <si>
+    <t>6.10.2</t>
+  </si>
+  <si>
+    <t>{Rescue Therapy}</t>
+  </si>
+  <si>
+    <t>6.10.3</t>
+  </si>
+  <si>
+    <t>{Other Non-investigational Intervention}</t>
+  </si>
+  <si>
+    <t>6.11</t>
+  </si>
+  <si>
+    <t>6.11.1</t>
+  </si>
+  <si>
+    <t>{Prohibited Concomitant Therapy}</t>
+  </si>
+  <si>
+    <t>6.11.2</t>
+  </si>
+  <si>
+    <t>{Permitted Concomitant Therapy}</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>PARTICIPANT DISCONTINUATION OF TRIAL INTERVENTION AND DISCONTINUATION OR WITHDRAWAL FROM TRIAL</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>Discontinuation of Trial Intervention for Individual Participants</t>
+  </si>
+  <si>
+    <t>7.1.1</t>
+  </si>
+  <si>
+    <t>Permanent Discontinuation of Trial Intervention</t>
+  </si>
+  <si>
+    <t>7.1.2</t>
+  </si>
+  <si>
+    <t>Temporary Discontinuation of Trial Intervention</t>
+  </si>
+  <si>
+    <t>7.1.3</t>
+  </si>
+  <si>
+    <t>Rechallenge</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>Discontinuation or Withdrawal from the Trial</t>
+  </si>
+  <si>
+    <t>7.3</t>
+  </si>
+  <si>
+    <t>Lost to Follow-Up</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>TRIAL ASSESSMENTS AND PROCEDURES</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>Trial Assessments and Procedures Considerations</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>Screening/Baseline Assessments and Procedures</t>
+  </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
+    <t>Efficacy Assessments and Procedures</t>
+  </si>
+  <si>
+    <t>8.4</t>
+  </si>
+  <si>
+    <t>Safety Assessments and Procedures</t>
+  </si>
+  <si>
+    <t>8.4.1</t>
+  </si>
+  <si>
+    <t>{Physical Examination}</t>
+  </si>
+  <si>
+    <t>8.4.2</t>
+  </si>
+  <si>
+    <t>{Vital Signs}</t>
+  </si>
+  <si>
+    <t>8.4.3</t>
+  </si>
+  <si>
+    <t>{Electrocardiograms}</t>
+  </si>
+  <si>
+    <t>8.4.4</t>
+  </si>
+  <si>
+    <t>{Clinical Laboratory Assessments}</t>
+  </si>
+  <si>
+    <t>8.4.5</t>
+  </si>
+  <si>
+    <t>{Pregnancy Testing}</t>
+  </si>
+  <si>
+    <t>8.4.6</t>
+  </si>
+  <si>
+    <t>{Suicidal Ideation and Behaviour Risk Monitoring}</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>8.6</t>
+  </si>
+  <si>
+    <t>Biomarkers</t>
+  </si>
+  <si>
+    <t>8.6.1</t>
+  </si>
+  <si>
+    <t>Genetics and Pharmacogenomics</t>
+  </si>
+  <si>
+    <t>8.6.2</t>
+  </si>
+  <si>
+    <t>Pharmacodynamic Biomarkers</t>
+  </si>
+  <si>
+    <t>8.6.3</t>
+  </si>
+  <si>
+    <t>{Other Biomarkers}</t>
+  </si>
+  <si>
+    <t>8.7</t>
+  </si>
+  <si>
+    <t>Immunogenicity Assessments</t>
+  </si>
+  <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>Medical Resource Utilisation and Health Economics</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>ADVERSE EVENTS,SERIOUS ADVERSE EVENTS,PRODUCT COMPLAINTS,PREGNANCY AND POSTPARTUM INFORMATION</t>
+  </si>
+  <si>
+    <t>9.1</t>
+  </si>
+  <si>
+    <t>Definitions</t>
+  </si>
+  <si>
+    <t>9.1.1</t>
+  </si>
+  <si>
+    <t>Definitions of Adverse Events</t>
+  </si>
+  <si>
+    <t>9.1.2</t>
+  </si>
+  <si>
+    <t>Definitions of Serious Adverse Events</t>
+  </si>
+  <si>
+    <t>9.1.3</t>
+  </si>
+  <si>
+    <t>{Definition of Medical Device Product Complaints}</t>
+  </si>
+  <si>
+    <t>9.2</t>
+  </si>
+  <si>
+    <t>Timing and Mechanism for Collection and Reporting</t>
+  </si>
+  <si>
+    <t>9.3</t>
+  </si>
+  <si>
+    <t>Identification,Recording and Follow-Up</t>
+  </si>
+  <si>
+    <t>9.3.1</t>
+  </si>
+  <si>
+    <t>Identification</t>
+  </si>
+  <si>
+    <t>9.3.2</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>9.3.3</t>
+  </si>
+  <si>
+    <t>Causality</t>
+  </si>
+  <si>
+    <t>9.3.4</t>
+  </si>
+  <si>
+    <t>Follow-up</t>
+  </si>
+  <si>
+    <t>9.4</t>
+  </si>
+  <si>
+    <t>Reporting</t>
+  </si>
+  <si>
+    <t>9.4.1</t>
+  </si>
+  <si>
+    <t>Regulatory Reporting Requirements</t>
+  </si>
+  <si>
+    <t>9.4.2</t>
+  </si>
+  <si>
+    <t>Adverse Events of Special Interest</t>
+  </si>
+  <si>
+    <t>9.4.3</t>
+  </si>
+  <si>
+    <t>Disease-related Events or Outcomes Not Qualifying as AEs or SAEs</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>Pregnancy and Postpartum Information</t>
+  </si>
+  <si>
+    <t>9.5.1</t>
+  </si>
+  <si>
+    <t>{Participants Who Become Pregnant During the Trial}</t>
+  </si>
+  <si>
+    <t>9.5.2</t>
+  </si>
+  <si>
+    <t>{Participants Whose Partners Become Pregnant}</t>
+  </si>
+  <si>
+    <t>STATISTICAL CONSIDERATIONS</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>10.2</t>
+  </si>
+  <si>
+    <t>Analysis Sets</t>
+  </si>
+  <si>
+    <t>10.3</t>
+  </si>
+  <si>
+    <t>Analyses of Demographics and Other Baseline Variables</t>
+  </si>
+  <si>
+    <t>10.4</t>
+  </si>
+  <si>
+    <t>Analyses Associated with the Primary Objective(s)</t>
+  </si>
+  <si>
+    <t>10.4.1</t>
+  </si>
+  <si>
+    <t>Statistical Method of Analysis</t>
+  </si>
+  <si>
+    <t>10.4.2</t>
+  </si>
+  <si>
+    <t>Handling of Data in Relation to Primary Estimand(s)</t>
+  </si>
+  <si>
+    <t>10.4.3</t>
+  </si>
+  <si>
+    <t>Handling of Missing Data</t>
+  </si>
+  <si>
+    <t>10.4.4</t>
+  </si>
+  <si>
+    <t>{Sensitivity Analysis}</t>
+  </si>
+  <si>
+    <t>10.4.5</t>
+  </si>
+  <si>
+    <t>{Supplementary Analysis}</t>
+  </si>
+  <si>
+    <t>10.5</t>
+  </si>
+  <si>
+    <t>Analysis Associated with the Secondary Objective(s)</t>
+  </si>
+  <si>
+    <t>10.5.1</t>
+  </si>
+  <si>
+    <t>{Statistical Method of Analysis}</t>
+  </si>
+  <si>
+    <t>10.5.2</t>
+  </si>
+  <si>
+    <t>{Handling of Data in Relation to Secondary Estimand(s)}</t>
+  </si>
+  <si>
+    <t>10.5.3</t>
+  </si>
+  <si>
+    <t>{Handling of Missing Data}</t>
+  </si>
+  <si>
+    <t>10.5.4</t>
+  </si>
+  <si>
+    <t>{Sensitivity Analyses}</t>
+  </si>
+  <si>
+    <t>10.5.5</t>
+  </si>
+  <si>
+    <t>{Supplementary Analyses}</t>
+  </si>
+  <si>
+    <t>10.6</t>
+  </si>
+  <si>
+    <t>Analysis Associated with the Exploratory Objective(s)</t>
+  </si>
+  <si>
+    <t>10.7</t>
+  </si>
+  <si>
+    <t>10.8</t>
+  </si>
+  <si>
+    <t>Other Analyses</t>
+  </si>
+  <si>
+    <t>10.9</t>
+  </si>
+  <si>
+    <t>Interim Analyses</t>
+  </si>
+  <si>
+    <t>10.10</t>
+  </si>
+  <si>
+    <t>Multiplicity Adjustments</t>
+  </si>
+  <si>
+    <t>10.11</t>
+  </si>
+  <si>
+    <t>Sample Size Determination</t>
+  </si>
+  <si>
+    <t>TRIAL OVERSIGHT AND OTHER GENERAL CONSIDERATIONS</t>
+  </si>
+  <si>
+    <t>11.1</t>
+  </si>
+  <si>
+    <t>Regulatory and Ethical Considerations</t>
+  </si>
+  <si>
+    <t>11.2</t>
+  </si>
+  <si>
+    <t>Trial Oversight</t>
+  </si>
+  <si>
+    <t>11.2.1</t>
+  </si>
+  <si>
+    <t>Investigator Responsibilities</t>
+  </si>
+  <si>
+    <t>11.2.2</t>
+  </si>
+  <si>
+    <t>Sponsor Responsibilities</t>
+  </si>
+  <si>
+    <t>11.3</t>
+  </si>
+  <si>
+    <t>Informed Consent Process</t>
+  </si>
+  <si>
+    <t>11.3.1</t>
+  </si>
+  <si>
+    <t>Informed Consent for Rescreening</t>
+  </si>
+  <si>
+    <t>11.3.2</t>
+  </si>
+  <si>
+    <t>Informed Consent for Use of Remaining Samples in Exploratory Research</t>
+  </si>
+  <si>
+    <t>11.4</t>
+  </si>
+  <si>
+    <t>Committees</t>
+  </si>
+  <si>
+    <t>11.5</t>
+  </si>
+  <si>
+    <t>Insurance and Indemnity</t>
+  </si>
+  <si>
+    <t>11.6</t>
+  </si>
+  <si>
+    <t>Risk Management</t>
+  </si>
+  <si>
+    <t>11.7</t>
+  </si>
+  <si>
+    <t>Data Governance</t>
+  </si>
+  <si>
+    <t>11.8</t>
+  </si>
+  <si>
+    <t>Source Data</t>
+  </si>
+  <si>
+    <t>11.9</t>
+  </si>
+  <si>
+    <t>Protocol Deviations</t>
+  </si>
+  <si>
+    <t>11.10</t>
+  </si>
+  <si>
+    <t>Early Site Closure</t>
+  </si>
+  <si>
+    <t>APPENDIX: SUPPORTING DETAILS</t>
+  </si>
+  <si>
+    <t>12.1</t>
+  </si>
+  <si>
+    <t>12.2</t>
+  </si>
+  <si>
+    <t>Country/Region-Specific Differences</t>
+  </si>
+  <si>
+    <t>12.3</t>
+  </si>
+  <si>
+    <t>Prior Protocol Amendment(s)</t>
+  </si>
+  <si>
+    <t>APPENDIX:  GLOSSARY OF TERMS AND ABBREVIATIONS</t>
+  </si>
+  <si>
+    <t>APPENDIX:  REFERENCES</t>
+  </si>
+  <si>
+    <t>lilly=lillyFormat</t>
+  </si>
+  <si>
+    <t>lilly</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>Use Template</t>
+  </si>
+  <si>
+    <t>m11=m11Format</t>
+  </si>
 </sst>
 </file>
 
@@ -4917,12 +5840,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -5094,6 +6020,12 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -5107,10 +6039,11 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{1568E383-B2B1-5645-AB16-743AC8157926}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -8693,7 +9626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9162AE3F-0A5D-824F-8BC1-E6A493EFAA49}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -9969,7 +10902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView topLeftCell="C28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -10063,7 +10996,7 @@
       </c>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A8" s="48" t="s">
         <v>603</v>
       </c>
@@ -10075,7 +11008,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A9" s="48" t="s">
         <v>606</v>
       </c>
@@ -10087,7 +11020,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="48" t="s">
         <v>609</v>
       </c>
@@ -10099,7 +11032,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="48" t="s">
         <v>612</v>
       </c>
@@ -10121,7 +11054,7 @@
       </c>
       <c r="D12" s="13"/>
     </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="48" t="s">
         <v>617</v>
       </c>
@@ -10169,7 +11102,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="48" t="s">
         <v>627</v>
       </c>
@@ -10193,7 +11126,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="48" t="s">
         <v>633</v>
       </c>
@@ -10227,7 +11160,7 @@
       </c>
       <c r="D21" s="13"/>
     </row>
-    <row r="22" spans="1:4" ht="255" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="187" x14ac:dyDescent="0.2">
       <c r="A22" s="48" t="s">
         <v>641</v>
       </c>
@@ -10239,7 +11172,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A23" s="48" t="s">
         <v>644</v>
       </c>
@@ -10251,7 +11184,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="136" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A24" s="48" t="s">
         <v>647</v>
       </c>
@@ -10309,7 +11242,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A29" s="48" t="s">
         <v>660</v>
       </c>
@@ -10900,13 +11833,1609 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED6534B-B4C9-924A-BB14-180C2C37C6F1}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E75AA97-4922-F248-8DDB-BFD2366D5770}">
+  <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="14.83203125" style="61" customWidth="1"/>
+    <col min="2" max="2" width="9" style="61" customWidth="1"/>
+    <col min="3" max="3" width="58.6640625" style="62" customWidth="1"/>
+    <col min="4" max="4" width="130.1640625" style="61" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="44" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="47" t="s">
+        <v>877</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="46" t="s">
+        <v>878</v>
+      </c>
+      <c r="D2" s="46"/>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="46" t="s">
+        <v>879</v>
+      </c>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46" t="s">
+        <v>880</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="46" t="s">
+        <v>882</v>
+      </c>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46" t="s">
+        <v>883</v>
+      </c>
+      <c r="D4" s="46"/>
+    </row>
+    <row r="5" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5" s="46" t="s">
+        <v>884</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46" t="s">
+        <v>885</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="46" t="s">
+        <v>887</v>
+      </c>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46" t="s">
+        <v>888</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="46" t="s">
+        <v>890</v>
+      </c>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46" t="s">
+        <v>891</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46" t="s">
+        <v>892</v>
+      </c>
+      <c r="D8" s="46"/>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="46" t="s">
+        <v>893</v>
+      </c>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46" t="s">
+        <v>894</v>
+      </c>
+      <c r="D9" s="46"/>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="46" t="s">
+        <v>895</v>
+      </c>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46" t="s">
+        <v>896</v>
+      </c>
+      <c r="D10" s="46"/>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="46" t="s">
+        <v>897</v>
+      </c>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46" t="s">
+        <v>898</v>
+      </c>
+      <c r="D11" s="46"/>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="46" t="s">
+        <v>899</v>
+      </c>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46" t="s">
+        <v>900</v>
+      </c>
+      <c r="D12" s="46"/>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="46" t="s">
+        <v>901</v>
+      </c>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46" t="s">
+        <v>902</v>
+      </c>
+      <c r="D13" s="46"/>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="46" t="s">
+        <v>903</v>
+      </c>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46" t="s">
+        <v>904</v>
+      </c>
+      <c r="D14" s="46"/>
+    </row>
+    <row r="15" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A15" s="46" t="s">
+        <v>905</v>
+      </c>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46" t="s">
+        <v>906</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="46" t="s">
+        <v>907</v>
+      </c>
+      <c r="B16" s="46"/>
+      <c r="C16" s="46" t="s">
+        <v>908</v>
+      </c>
+      <c r="D16" s="46"/>
+    </row>
+    <row r="17" spans="1:4" ht="119" x14ac:dyDescent="0.2">
+      <c r="A17" s="46" t="s">
+        <v>909</v>
+      </c>
+      <c r="B17" s="46"/>
+      <c r="C17" s="46" t="s">
+        <v>910</v>
+      </c>
+      <c r="D17" s="46" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="46" t="s">
+        <v>911</v>
+      </c>
+      <c r="B18" s="46"/>
+      <c r="C18" s="46" t="s">
+        <v>912</v>
+      </c>
+      <c r="D18" s="46"/>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="46" t="s">
+        <v>913</v>
+      </c>
+      <c r="B19" s="46"/>
+      <c r="C19" s="46" t="s">
+        <v>914</v>
+      </c>
+      <c r="D19" s="46"/>
+    </row>
+    <row r="20" spans="1:4" ht="221" x14ac:dyDescent="0.2">
+      <c r="A20" s="46" t="s">
+        <v>915</v>
+      </c>
+      <c r="B20" s="46"/>
+      <c r="C20" s="46" t="s">
+        <v>916</v>
+      </c>
+      <c r="D20" s="46" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="46" t="s">
+        <v>918</v>
+      </c>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46" t="s">
+        <v>919</v>
+      </c>
+      <c r="D21" s="46"/>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="46" t="s">
+        <v>920</v>
+      </c>
+      <c r="B22" s="46"/>
+      <c r="C22" s="46" t="s">
+        <v>921</v>
+      </c>
+      <c r="D22" s="46"/>
+    </row>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="46" t="s">
+        <v>922</v>
+      </c>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46" t="s">
+        <v>923</v>
+      </c>
+      <c r="D23" s="46"/>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="46" t="s">
+        <v>924</v>
+      </c>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46" t="s">
+        <v>925</v>
+      </c>
+      <c r="D24" s="46"/>
+    </row>
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="46" t="s">
+        <v>926</v>
+      </c>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46" t="s">
+        <v>927</v>
+      </c>
+      <c r="D25" s="46"/>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="46" t="s">
+        <v>928</v>
+      </c>
+      <c r="B26" s="46"/>
+      <c r="C26" s="46" t="s">
+        <v>929</v>
+      </c>
+      <c r="D26" s="46"/>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="46" t="s">
+        <v>930</v>
+      </c>
+      <c r="B27" s="46"/>
+      <c r="C27" s="46" t="s">
+        <v>931</v>
+      </c>
+      <c r="D27" s="46"/>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="46" t="s">
+        <v>932</v>
+      </c>
+      <c r="B28" s="46"/>
+      <c r="C28" s="46" t="s">
+        <v>933</v>
+      </c>
+      <c r="D28" s="46"/>
+    </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="46" t="s">
+        <v>934</v>
+      </c>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46" t="s">
+        <v>935</v>
+      </c>
+      <c r="D29" s="46"/>
+    </row>
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="46" t="s">
+        <v>936</v>
+      </c>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46" t="s">
+        <v>937</v>
+      </c>
+      <c r="D30" s="46"/>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="46" t="s">
+        <v>938</v>
+      </c>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46" t="s">
+        <v>939</v>
+      </c>
+      <c r="D31" s="46"/>
+    </row>
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="46" t="s">
+        <v>940</v>
+      </c>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46" t="s">
+        <v>941</v>
+      </c>
+      <c r="D32" s="46"/>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="46" t="s">
+        <v>942</v>
+      </c>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46" t="s">
+        <v>943</v>
+      </c>
+      <c r="D33" s="46"/>
+    </row>
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="46" t="s">
+        <v>944</v>
+      </c>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46" t="s">
+        <v>945</v>
+      </c>
+      <c r="D34" s="46"/>
+    </row>
+    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="46" t="s">
+        <v>946</v>
+      </c>
+      <c r="B35" s="46"/>
+      <c r="C35" s="46" t="s">
+        <v>623</v>
+      </c>
+      <c r="D35" s="46" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A36" s="46" t="s">
+        <v>947</v>
+      </c>
+      <c r="B36" s="46"/>
+      <c r="C36" s="46" t="s">
+        <v>626</v>
+      </c>
+      <c r="D36" s="46" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="46" t="s">
+        <v>948</v>
+      </c>
+      <c r="B37" s="46"/>
+      <c r="C37" s="46" t="s">
+        <v>949</v>
+      </c>
+      <c r="D37" s="46"/>
+    </row>
+    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="46" t="s">
+        <v>950</v>
+      </c>
+      <c r="B38" s="46"/>
+      <c r="C38" s="46" t="s">
+        <v>951</v>
+      </c>
+      <c r="D38" s="46"/>
+    </row>
+    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="46" t="s">
+        <v>952</v>
+      </c>
+      <c r="B39" s="46"/>
+      <c r="C39" s="46" t="s">
+        <v>953</v>
+      </c>
+      <c r="D39" s="46"/>
+    </row>
+    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="46" t="s">
+        <v>954</v>
+      </c>
+      <c r="B40" s="46"/>
+      <c r="C40" s="46" t="s">
+        <v>955</v>
+      </c>
+      <c r="D40" s="46"/>
+    </row>
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="46" t="s">
+        <v>956</v>
+      </c>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46" t="s">
+        <v>957</v>
+      </c>
+      <c r="D41" s="46"/>
+    </row>
+    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="46" t="s">
+        <v>958</v>
+      </c>
+      <c r="B42" s="46"/>
+      <c r="C42" s="46" t="s">
+        <v>959</v>
+      </c>
+      <c r="D42" s="46"/>
+    </row>
+    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="46" t="s">
+        <v>960</v>
+      </c>
+      <c r="B43" s="46"/>
+      <c r="C43" s="46" t="s">
+        <v>961</v>
+      </c>
+      <c r="D43" s="46"/>
+    </row>
+    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="46" t="s">
+        <v>962</v>
+      </c>
+      <c r="B44" s="46"/>
+      <c r="C44" s="46" t="s">
+        <v>963</v>
+      </c>
+      <c r="D44" s="46"/>
+    </row>
+    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="46" t="s">
+        <v>964</v>
+      </c>
+      <c r="B45" s="46"/>
+      <c r="C45" s="46" t="s">
+        <v>965</v>
+      </c>
+      <c r="D45" s="46"/>
+    </row>
+    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="46" t="s">
+        <v>966</v>
+      </c>
+      <c r="B46" s="46"/>
+      <c r="C46" s="46" t="s">
+        <v>967</v>
+      </c>
+      <c r="D46" s="46"/>
+    </row>
+    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="46" t="s">
+        <v>968</v>
+      </c>
+      <c r="B47" s="46"/>
+      <c r="C47" s="46" t="s">
+        <v>969</v>
+      </c>
+      <c r="D47" s="46"/>
+    </row>
+    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="46" t="s">
+        <v>970</v>
+      </c>
+      <c r="B48" s="46"/>
+      <c r="C48" s="46" t="s">
+        <v>971</v>
+      </c>
+      <c r="D48" s="46"/>
+    </row>
+    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="46" t="s">
+        <v>972</v>
+      </c>
+      <c r="B49" s="46"/>
+      <c r="C49" s="46" t="s">
+        <v>973</v>
+      </c>
+      <c r="D49" s="46"/>
+    </row>
+    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="46" t="s">
+        <v>974</v>
+      </c>
+      <c r="B50" s="46"/>
+      <c r="C50" s="46" t="s">
+        <v>975</v>
+      </c>
+      <c r="D50" s="46"/>
+    </row>
+    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="46" t="s">
+        <v>976</v>
+      </c>
+      <c r="B51" s="46"/>
+      <c r="C51" s="46" t="s">
+        <v>977</v>
+      </c>
+      <c r="D51" s="46"/>
+    </row>
+    <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="46" t="s">
+        <v>978</v>
+      </c>
+      <c r="B52" s="46"/>
+      <c r="C52" s="46" t="s">
+        <v>979</v>
+      </c>
+      <c r="D52" s="46"/>
+    </row>
+    <row r="53" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A53" s="46" t="s">
+        <v>980</v>
+      </c>
+      <c r="B53" s="46"/>
+      <c r="C53" s="46" t="s">
+        <v>981</v>
+      </c>
+      <c r="D53" s="46"/>
+    </row>
+    <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="46" t="s">
+        <v>982</v>
+      </c>
+      <c r="B54" s="46"/>
+      <c r="C54" s="46" t="s">
+        <v>983</v>
+      </c>
+      <c r="D54" s="46"/>
+    </row>
+    <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="46" t="s">
+        <v>984</v>
+      </c>
+      <c r="B55" s="46"/>
+      <c r="C55" s="46" t="s">
+        <v>985</v>
+      </c>
+      <c r="D55" s="46"/>
+    </row>
+    <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="46" t="s">
+        <v>986</v>
+      </c>
+      <c r="B56" s="46"/>
+      <c r="C56" s="46" t="s">
+        <v>987</v>
+      </c>
+      <c r="D56" s="46"/>
+    </row>
+    <row r="57" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A57" s="46" t="s">
+        <v>988</v>
+      </c>
+      <c r="B57" s="46"/>
+      <c r="C57" s="46" t="s">
+        <v>989</v>
+      </c>
+      <c r="D57" s="46"/>
+    </row>
+    <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="46" t="s">
+        <v>990</v>
+      </c>
+      <c r="B58" s="46"/>
+      <c r="C58" s="46" t="s">
+        <v>991</v>
+      </c>
+      <c r="D58" s="46"/>
+    </row>
+    <row r="59" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="46" t="s">
+        <v>992</v>
+      </c>
+      <c r="B59" s="46"/>
+      <c r="C59" s="46" t="s">
+        <v>993</v>
+      </c>
+      <c r="D59" s="46"/>
+    </row>
+    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="46" t="s">
+        <v>994</v>
+      </c>
+      <c r="B60" s="46"/>
+      <c r="C60" s="46" t="s">
+        <v>995</v>
+      </c>
+      <c r="D60" s="46"/>
+    </row>
+    <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="46" t="s">
+        <v>996</v>
+      </c>
+      <c r="B61" s="46"/>
+      <c r="C61" s="46" t="s">
+        <v>997</v>
+      </c>
+      <c r="D61" s="46"/>
+    </row>
+    <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="46" t="s">
+        <v>998</v>
+      </c>
+      <c r="B62" s="46"/>
+      <c r="C62" s="46" t="s">
+        <v>999</v>
+      </c>
+      <c r="D62" s="46"/>
+    </row>
+    <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="46" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B63" s="46"/>
+      <c r="C63" s="46" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D63" s="46"/>
+    </row>
+    <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="46" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B64" s="46"/>
+      <c r="C64" s="46" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D64" s="46"/>
+    </row>
+    <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="46" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B65" s="46"/>
+      <c r="C65" s="46" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D65" s="46"/>
+    </row>
+    <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="46" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B66" s="46"/>
+      <c r="C66" s="46" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D66" s="46"/>
+    </row>
+    <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="46" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B67" s="46"/>
+      <c r="C67" s="46" t="s">
+        <v>651</v>
+      </c>
+      <c r="D67" s="46"/>
+    </row>
+    <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="46" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B68" s="46"/>
+      <c r="C68" s="46" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D68" s="46"/>
+    </row>
+    <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="46" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B69" s="46"/>
+      <c r="C69" s="46" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D69" s="46"/>
+    </row>
+    <row r="70" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A70" s="46" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B70" s="46"/>
+      <c r="C70" s="46" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D70" s="46"/>
+    </row>
+    <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="46" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B71" s="46"/>
+      <c r="C71" s="46" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D71" s="46"/>
+    </row>
+    <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A72" s="46" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B72" s="46"/>
+      <c r="C72" s="46" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D72" s="46"/>
+    </row>
+    <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" s="46" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B73" s="46"/>
+      <c r="C73" s="46" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D73" s="46"/>
+    </row>
+    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" s="46" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B74" s="46"/>
+      <c r="C74" s="46" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D74" s="46"/>
+    </row>
+    <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="46" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B75" s="46"/>
+      <c r="C75" s="46" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D75" s="46"/>
+    </row>
+    <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="46" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B76" s="46"/>
+      <c r="C76" s="46" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D76" s="46"/>
+    </row>
+    <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A77" s="46" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B77" s="46"/>
+      <c r="C77" s="46" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D77" s="46"/>
+    </row>
+    <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="46" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B78" s="46"/>
+      <c r="C78" s="46" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D78" s="46"/>
+    </row>
+    <row r="79" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="46" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B79" s="46"/>
+      <c r="C79" s="46" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D79" s="46"/>
+    </row>
+    <row r="80" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="46" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B80" s="46"/>
+      <c r="C80" s="46" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D80" s="46"/>
+    </row>
+    <row r="81" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" s="46" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B81" s="46"/>
+      <c r="C81" s="46" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D81" s="46"/>
+    </row>
+    <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="46" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B82" s="46"/>
+      <c r="C82" s="46" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D82" s="46"/>
+    </row>
+    <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" s="46" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B83" s="46"/>
+      <c r="C83" s="46" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D83" s="46"/>
+    </row>
+    <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A84" s="46" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B84" s="46"/>
+      <c r="C84" s="46" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D84" s="46"/>
+    </row>
+    <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="46" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B85" s="46"/>
+      <c r="C85" s="46" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D85" s="46"/>
+    </row>
+    <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A86" s="46" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B86" s="46"/>
+      <c r="C86" s="46" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D86" s="46"/>
+    </row>
+    <row r="87" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A87" s="46" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B87" s="46"/>
+      <c r="C87" s="46" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D87" s="46"/>
+    </row>
+    <row r="88" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A88" s="46" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B88" s="46"/>
+      <c r="C88" s="46" t="s">
+        <v>664</v>
+      </c>
+      <c r="D88" s="46"/>
+    </row>
+    <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A89" s="46" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B89" s="46"/>
+      <c r="C89" s="46" t="s">
+        <v>1051</v>
+      </c>
+      <c r="D89" s="46"/>
+    </row>
+    <row r="90" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A90" s="46" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B90" s="46"/>
+      <c r="C90" s="46" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D90" s="46"/>
+    </row>
+    <row r="91" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A91" s="46" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B91" s="46"/>
+      <c r="C91" s="46" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D91" s="46"/>
+    </row>
+    <row r="92" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A92" s="46" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B92" s="46"/>
+      <c r="C92" s="46" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D92" s="46"/>
+    </row>
+    <row r="93" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="46" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B93" s="46"/>
+      <c r="C93" s="46" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D93" s="46"/>
+    </row>
+    <row r="94" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A94" s="46" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B94" s="46"/>
+      <c r="C94" s="46" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D94" s="46"/>
+    </row>
+    <row r="95" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A95" s="46" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B95" s="46"/>
+      <c r="C95" s="46" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D95" s="46"/>
+    </row>
+    <row r="96" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="46" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B96" s="46"/>
+      <c r="C96" s="46" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D96" s="46"/>
+    </row>
+    <row r="97" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="46" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B97" s="46"/>
+      <c r="C97" s="46" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D97" s="46"/>
+    </row>
+    <row r="98" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="46" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B98" s="46"/>
+      <c r="C98" s="46" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D98" s="46"/>
+    </row>
+    <row r="99" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="46" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B99" s="46"/>
+      <c r="C99" s="46" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D99" s="46"/>
+    </row>
+    <row r="100" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="46" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B100" s="46"/>
+      <c r="C100" s="46" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D100" s="46"/>
+    </row>
+    <row r="101" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="46" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B101" s="46"/>
+      <c r="C101" s="46" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D101" s="46"/>
+    </row>
+    <row r="102" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="46" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B102" s="46"/>
+      <c r="C102" s="46" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D102" s="46"/>
+    </row>
+    <row r="103" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" s="46" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B103" s="46"/>
+      <c r="C103" s="46" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D103" s="46"/>
+    </row>
+    <row r="104" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" s="46" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B104" s="46"/>
+      <c r="C104" s="46" t="s">
+        <v>1081</v>
+      </c>
+      <c r="D104" s="46"/>
+    </row>
+    <row r="105" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" s="46" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B105" s="46"/>
+      <c r="C105" s="46" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D105" s="46"/>
+    </row>
+    <row r="106" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" s="46" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B106" s="46"/>
+      <c r="C106" s="46" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D106" s="46"/>
+    </row>
+    <row r="107" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" s="46" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B107" s="46"/>
+      <c r="C107" s="46" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D107" s="46"/>
+    </row>
+    <row r="108" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="46" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B108" s="46"/>
+      <c r="C108" s="46" t="s">
+        <v>1089</v>
+      </c>
+      <c r="D108" s="46"/>
+    </row>
+    <row r="109" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="46" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B109" s="46"/>
+      <c r="C109" s="46" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D109" s="46"/>
+    </row>
+    <row r="110" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="46" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B110" s="46"/>
+      <c r="C110" s="46" t="s">
+        <v>1093</v>
+      </c>
+      <c r="D110" s="46"/>
+    </row>
+    <row r="111" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="46" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B111" s="46"/>
+      <c r="C111" s="46" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D111" s="46"/>
+    </row>
+    <row r="112" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="46" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B112" s="46"/>
+      <c r="C112" s="46" t="s">
+        <v>1097</v>
+      </c>
+      <c r="D112" s="46"/>
+    </row>
+    <row r="113" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A113" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="B113" s="46"/>
+      <c r="C113" s="46" t="s">
+        <v>1098</v>
+      </c>
+      <c r="D113" s="46"/>
+    </row>
+    <row r="114" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A114" s="46" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B114" s="46"/>
+      <c r="C114" s="46" t="s">
+        <v>718</v>
+      </c>
+      <c r="D114" s="46"/>
+    </row>
+    <row r="115" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A115" s="46" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B115" s="46"/>
+      <c r="C115" s="46" t="s">
+        <v>1101</v>
+      </c>
+      <c r="D115" s="46"/>
+    </row>
+    <row r="116" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" s="46" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B116" s="46"/>
+      <c r="C116" s="46" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D116" s="46"/>
+    </row>
+    <row r="117" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A117" s="46" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B117" s="46"/>
+      <c r="C117" s="46" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D117" s="46"/>
+    </row>
+    <row r="118" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A118" s="46" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B118" s="46"/>
+      <c r="C118" s="46" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D118" s="46"/>
+    </row>
+    <row r="119" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A119" s="46" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B119" s="46"/>
+      <c r="C119" s="46" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D119" s="46"/>
+    </row>
+    <row r="120" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A120" s="46" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B120" s="46"/>
+      <c r="C120" s="46" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D120" s="46"/>
+    </row>
+    <row r="121" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A121" s="46" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B121" s="46"/>
+      <c r="C121" s="46" t="s">
+        <v>1113</v>
+      </c>
+      <c r="D121" s="46"/>
+    </row>
+    <row r="122" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A122" s="46" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B122" s="46"/>
+      <c r="C122" s="46" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D122" s="46"/>
+    </row>
+    <row r="123" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A123" s="46" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B123" s="46"/>
+      <c r="C123" s="46" t="s">
+        <v>1117</v>
+      </c>
+      <c r="D123" s="46"/>
+    </row>
+    <row r="124" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A124" s="46" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B124" s="46"/>
+      <c r="C124" s="46" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D124" s="46"/>
+    </row>
+    <row r="125" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A125" s="46" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B125" s="46"/>
+      <c r="C125" s="46" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D125" s="46"/>
+    </row>
+    <row r="126" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A126" s="46" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B126" s="46"/>
+      <c r="C126" s="46" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D126" s="46"/>
+    </row>
+    <row r="127" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A127" s="46" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B127" s="46"/>
+      <c r="C127" s="46" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D127" s="46"/>
+    </row>
+    <row r="128" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A128" s="46" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B128" s="46"/>
+      <c r="C128" s="46" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D128" s="46"/>
+    </row>
+    <row r="129" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A129" s="46" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B129" s="46"/>
+      <c r="C129" s="46" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D129" s="46"/>
+    </row>
+    <row r="130" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A130" s="46" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B130" s="46"/>
+      <c r="C130" s="46" t="s">
+        <v>741</v>
+      </c>
+      <c r="D130" s="46"/>
+    </row>
+    <row r="131" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A131" s="46" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B131" s="46"/>
+      <c r="C131" s="46" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D131" s="46"/>
+    </row>
+    <row r="132" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A132" s="46" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B132" s="46"/>
+      <c r="C132" s="46" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D132" s="46"/>
+    </row>
+    <row r="133" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A133" s="46" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B133" s="46"/>
+      <c r="C133" s="46" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D133" s="46"/>
+    </row>
+    <row r="134" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A134" s="46" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B134" s="46"/>
+      <c r="C134" s="46" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D134" s="46"/>
+    </row>
+    <row r="135" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A135" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="B135" s="46"/>
+      <c r="C135" s="46" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D135" s="46"/>
+    </row>
+    <row r="136" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A136" s="46" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B136" s="46"/>
+      <c r="C136" s="46" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D136" s="46"/>
+    </row>
+    <row r="137" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A137" s="46" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B137" s="46"/>
+      <c r="C137" s="46" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D137" s="46"/>
+    </row>
+    <row r="138" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A138" s="46" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B138" s="46"/>
+      <c r="C138" s="46" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D138" s="46"/>
+    </row>
+    <row r="139" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A139" s="46" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B139" s="46"/>
+      <c r="C139" s="46" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D139" s="46"/>
+    </row>
+    <row r="140" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A140" s="46" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B140" s="46"/>
+      <c r="C140" s="46" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D140" s="46"/>
+    </row>
+    <row r="141" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A141" s="46" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B141" s="46"/>
+      <c r="C141" s="46" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D141" s="46"/>
+    </row>
+    <row r="142" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A142" s="46" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B142" s="46"/>
+      <c r="C142" s="46" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D142" s="46"/>
+    </row>
+    <row r="143" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A143" s="46" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B143" s="46"/>
+      <c r="C143" s="46" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D143" s="46"/>
+    </row>
+    <row r="144" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A144" s="46" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B144" s="46"/>
+      <c r="C144" s="46" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D144" s="46"/>
+    </row>
+    <row r="145" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A145" s="46" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B145" s="46"/>
+      <c r="C145" s="46" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D145" s="46"/>
+    </row>
+    <row r="146" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A146" s="46" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B146" s="46"/>
+      <c r="C146" s="46" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D146" s="46"/>
+    </row>
+    <row r="147" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A147" s="46" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B147" s="46"/>
+      <c r="C147" s="46" t="s">
+        <v>1163</v>
+      </c>
+      <c r="D147" s="46"/>
+    </row>
+    <row r="148" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A148" s="46" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B148" s="46"/>
+      <c r="C148" s="46" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D148" s="46"/>
+    </row>
+    <row r="149" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A149" s="46" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B149" s="46"/>
+      <c r="C149" s="46" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D149" s="46"/>
+    </row>
+    <row r="150" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A150" s="46" t="s">
+        <v>228</v>
+      </c>
+      <c r="B150" s="46"/>
+      <c r="C150" s="46" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D150" s="46"/>
+    </row>
+    <row r="151" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A151" s="46" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B151" s="46"/>
+      <c r="C151" s="46" t="s">
+        <v>681</v>
+      </c>
+      <c r="D151" s="46"/>
+    </row>
+    <row r="152" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A152" s="46" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B152" s="46"/>
+      <c r="C152" s="46" t="s">
+        <v>1171</v>
+      </c>
+      <c r="D152" s="46"/>
+    </row>
+    <row r="153" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A153" s="46" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B153" s="46"/>
+      <c r="C153" s="46" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D153" s="46"/>
+    </row>
+    <row r="154" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A154" s="46" t="s">
+        <v>229</v>
+      </c>
+      <c r="B154" s="46"/>
+      <c r="C154" s="46" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D154" s="46"/>
+    </row>
+    <row r="155" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A155" s="46" t="s">
+        <v>230</v>
+      </c>
+      <c r="B155" s="46"/>
+      <c r="C155" s="46" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D155" s="46"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED6534B-B4C9-924A-BB14-180C2C37C6F1}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10940,6 +13469,30 @@
       </c>
       <c r="B4" t="s">
         <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1177</v>
       </c>
     </row>
   </sheetData>
@@ -11051,144 +13604,144 @@
       <c r="A1" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="64" t="s">
         <v>534</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
     </row>
     <row r="4" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="65" t="s">
         <v>419</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
       <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>525</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="63" t="s">
         <v>526</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>527</v>
       </c>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="63" t="s">
         <v>528</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
+      <c r="C11" s="63"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="66" t="s">
         <v>437</v>
       </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Small tweak to config sheet
</commit_message>
<xml_diff>
--- a/source_data/protocols/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/protocols/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/protocols/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6911F1-6B83-6141-8BEF-AEBC921656D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9725F3AE-F9BB-B940-8DAD-43D01C5AE5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28700" yWindow="500" windowWidth="41180" windowHeight="27240" activeTab="12" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="59840" yWindow="500" windowWidth="41180" windowHeight="27240" firstSheet="15" activeTab="27" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3163" uniqueCount="1501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3161" uniqueCount="1499">
   <si>
     <t>Screening</t>
   </si>
@@ -4680,9 +4680,6 @@
   </si>
   <si>
     <t>Template</t>
-  </si>
-  <si>
-    <t>Use Template</t>
   </si>
   <si>
     <t>m11=m11Format</t>
@@ -5723,9 +5720,6 @@
 &lt;/ol&gt;</t>
   </si>
   <si>
-    <t>lilly</t>
-  </si>
-  <si>
     <t>NCI_1</t>
   </si>
   <si>
@@ -7009,18 +7003,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -7038,6 +7020,18 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -7058,6 +7052,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>262466</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1930400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>567266</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1279085</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C12D3F9C-EB68-FAF5-F932-136117464C2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16653933" y="6874933"/>
+          <a:ext cx="7772400" cy="6460685"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9108,7 +9151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B8B105-0AE3-CA42-845E-0FC79C427790}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="A19" sqref="A19:I19"/>
     </sheetView>
   </sheetViews>
@@ -11902,16 +11945,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.33203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="16.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="98.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -11921,25 +11965,25 @@
       <c r="B1" s="44" t="s">
         <v>221</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="62" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D1" s="63" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="62" t="s">
+        <v>1254</v>
+      </c>
+      <c r="F1" s="63" t="s">
         <v>1255</v>
-      </c>
-      <c r="D1" s="67" t="s">
-        <v>223</v>
-      </c>
-      <c r="E1" s="66" t="s">
-        <v>1256</v>
-      </c>
-      <c r="F1" s="67" t="s">
-        <v>1257</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="B2" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>500</v>
@@ -11947,16 +11991,16 @@
       <c r="D2" s="45" t="s">
         <v>590</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="64" t="s">
         <v>500</v>
       </c>
       <c r="F2" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="B3" t="s">
         <v>862</v>
@@ -11967,16 +12011,16 @@
       <c r="D3" s="45" t="s">
         <v>591</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F3" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="B4" t="s">
         <v>225</v>
@@ -11987,16 +12031,16 @@
       <c r="D4" s="45" t="s">
         <v>592</v>
       </c>
-      <c r="E4" s="68" t="s">
+      <c r="E4" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F4" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="B5" t="s">
         <v>593</v>
@@ -12007,16 +12051,16 @@
       <c r="D5" s="45" t="s">
         <v>594</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="E5" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F5" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="B6" t="s">
         <v>880</v>
@@ -12027,16 +12071,16 @@
       <c r="D6" s="45" t="s">
         <v>595</v>
       </c>
-      <c r="E6" s="68" t="s">
+      <c r="E6" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F6" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="B7" t="s">
         <v>888</v>
@@ -12047,16 +12091,16 @@
       <c r="D7" s="45" t="s">
         <v>596</v>
       </c>
-      <c r="E7" s="68" t="s">
+      <c r="E7" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F7" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="B8" t="s">
         <v>597</v>
@@ -12067,16 +12111,16 @@
       <c r="D8" s="45" t="s">
         <v>598</v>
       </c>
-      <c r="E8" s="68" t="s">
+      <c r="E8" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F8" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="B9" t="s">
         <v>600</v>
@@ -12087,16 +12131,16 @@
       <c r="D9" s="45" t="s">
         <v>601</v>
       </c>
-      <c r="E9" s="68" t="s">
+      <c r="E9" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F9" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="B10" t="s">
         <v>603</v>
@@ -12107,16 +12151,16 @@
       <c r="D10" s="45" t="s">
         <v>604</v>
       </c>
-      <c r="E10" s="68" t="s">
+      <c r="E10" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F10" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="B11" t="s">
         <v>606</v>
@@ -12127,16 +12171,16 @@
       <c r="D11" s="45" t="s">
         <v>607</v>
       </c>
-      <c r="E11" s="68" t="s">
+      <c r="E11" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F11" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="B12" t="s">
         <v>609</v>
@@ -12147,16 +12191,16 @@
       <c r="D12" s="45" t="s">
         <v>610</v>
       </c>
-      <c r="E12" s="68" t="s">
+      <c r="E12" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F12" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="B13" t="s">
         <v>611</v>
@@ -12167,16 +12211,16 @@
       <c r="D13" s="45" t="s">
         <v>612</v>
       </c>
-      <c r="E13" s="68" t="s">
+      <c r="E13" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F13" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="B14" t="s">
         <v>614</v>
@@ -12187,16 +12231,16 @@
       <c r="D14" s="45" t="s">
         <v>615</v>
       </c>
-      <c r="E14" s="68" t="s">
+      <c r="E14" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F14" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="B15" t="s">
         <v>616</v>
@@ -12207,16 +12251,16 @@
       <c r="D15" s="45" t="s">
         <v>617</v>
       </c>
-      <c r="E15" s="68" t="s">
+      <c r="E15" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F15" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="B16" t="s">
         <v>619</v>
@@ -12227,16 +12271,16 @@
       <c r="D16" s="45" t="s">
         <v>620</v>
       </c>
-      <c r="E16" s="68" t="s">
+      <c r="E16" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F16" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="B17" t="s">
         <v>621</v>
@@ -12247,16 +12291,16 @@
       <c r="D17" s="45" t="s">
         <v>622</v>
       </c>
-      <c r="E17" s="68" t="s">
+      <c r="E17" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F17" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="B18" t="s">
         <v>624</v>
@@ -12267,16 +12311,16 @@
       <c r="D18" s="45" t="s">
         <v>625</v>
       </c>
-      <c r="E18" s="68" t="s">
+      <c r="E18" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F18" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="B19" t="s">
         <v>627</v>
@@ -12287,16 +12331,16 @@
       <c r="D19" s="45" t="s">
         <v>628</v>
       </c>
-      <c r="E19" s="68" t="s">
+      <c r="E19" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F19" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="B20" t="s">
         <v>630</v>
@@ -12307,16 +12351,16 @@
       <c r="D20" s="45" t="s">
         <v>631</v>
       </c>
-      <c r="E20" s="68" t="s">
+      <c r="E20" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F20" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="B21" t="s">
         <v>633</v>
@@ -12327,16 +12371,16 @@
       <c r="D21" s="45" t="s">
         <v>634</v>
       </c>
-      <c r="E21" s="68" t="s">
+      <c r="E21" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F21" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="B22" t="s">
         <v>635</v>
@@ -12347,16 +12391,16 @@
       <c r="D22" s="45" t="s">
         <v>636</v>
       </c>
-      <c r="E22" s="68" t="s">
+      <c r="E22" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F22" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="B23" t="s">
         <v>638</v>
@@ -12367,16 +12411,16 @@
       <c r="D23" s="45" t="s">
         <v>639</v>
       </c>
-      <c r="E23" s="68" t="s">
+      <c r="E23" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F23" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="B24" t="s">
         <v>641</v>
@@ -12387,16 +12431,16 @@
       <c r="D24" s="45" t="s">
         <v>642</v>
       </c>
-      <c r="E24" s="68" t="s">
+      <c r="E24" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F24" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="B25" t="s">
         <v>644</v>
@@ -12407,16 +12451,16 @@
       <c r="D25" s="45" t="s">
         <v>645</v>
       </c>
-      <c r="E25" s="68" t="s">
+      <c r="E25" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F25" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="B26" t="s">
         <v>647</v>
@@ -12427,16 +12471,16 @@
       <c r="D26" s="45" t="s">
         <v>648</v>
       </c>
-      <c r="E26" s="68" t="s">
+      <c r="E26" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F26" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="B27" t="s">
         <v>649</v>
@@ -12447,16 +12491,16 @@
       <c r="D27" s="45" t="s">
         <v>650</v>
       </c>
-      <c r="E27" s="68" t="s">
+      <c r="E27" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F27" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="B28" t="s">
         <v>652</v>
@@ -12467,16 +12511,16 @@
       <c r="D28" s="45" t="s">
         <v>653</v>
       </c>
-      <c r="E28" s="68" t="s">
+      <c r="E28" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F28" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="B29" t="s">
         <v>654</v>
@@ -12487,16 +12531,16 @@
       <c r="D29" s="45" t="s">
         <v>655</v>
       </c>
-      <c r="E29" s="68" t="s">
+      <c r="E29" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F29" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="B30" t="s">
         <v>657</v>
@@ -12507,16 +12551,16 @@
       <c r="D30" s="45" t="s">
         <v>658</v>
       </c>
-      <c r="E30" s="68" t="s">
+      <c r="E30" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F30" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="B31" t="s">
         <v>660</v>
@@ -12527,16 +12571,16 @@
       <c r="D31" s="45" t="s">
         <v>343</v>
       </c>
-      <c r="E31" s="68" t="s">
+      <c r="E31" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F31" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="B32" t="s">
         <v>662</v>
@@ -12547,16 +12591,16 @@
       <c r="D32" s="45" t="s">
         <v>663</v>
       </c>
-      <c r="E32" s="68" t="s">
+      <c r="E32" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F32" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B33" t="s">
         <v>665</v>
@@ -12567,16 +12611,16 @@
       <c r="D33" s="45" t="s">
         <v>666</v>
       </c>
-      <c r="E33" s="68" t="s">
+      <c r="E33" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F33" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="B34" t="s">
         <v>668</v>
@@ -12587,16 +12631,16 @@
       <c r="D34" s="45" t="s">
         <v>669</v>
       </c>
-      <c r="E34" s="68" t="s">
+      <c r="E34" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F34" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="B35" t="s">
         <v>671</v>
@@ -12607,16 +12651,16 @@
       <c r="D35" s="45" t="s">
         <v>672</v>
       </c>
-      <c r="E35" s="68" t="s">
+      <c r="E35" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F35" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="B36" t="s">
         <v>674</v>
@@ -12627,16 +12671,16 @@
       <c r="D36" s="45" t="s">
         <v>675</v>
       </c>
-      <c r="E36" s="68" t="s">
+      <c r="E36" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F36" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="B37" t="s">
         <v>676</v>
@@ -12647,16 +12691,16 @@
       <c r="D37" s="45" t="s">
         <v>677</v>
       </c>
-      <c r="E37" s="68" t="s">
+      <c r="E37" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F37" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="B38" t="s">
         <v>678</v>
@@ -12667,16 +12711,16 @@
       <c r="D38" s="45" t="s">
         <v>679</v>
       </c>
-      <c r="E38" s="68" t="s">
+      <c r="E38" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F38" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="B39" t="s">
         <v>681</v>
@@ -12687,16 +12731,16 @@
       <c r="D39" s="45" t="s">
         <v>682</v>
       </c>
-      <c r="E39" s="68" t="s">
+      <c r="E39" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F39" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="B40" t="s">
         <v>684</v>
@@ -12707,16 +12751,16 @@
       <c r="D40" s="45" t="s">
         <v>685</v>
       </c>
-      <c r="E40" s="68" t="s">
+      <c r="E40" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F40" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="B41" t="s">
         <v>687</v>
@@ -12727,16 +12771,16 @@
       <c r="D41" s="45" t="s">
         <v>688</v>
       </c>
-      <c r="E41" s="68" t="s">
+      <c r="E41" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F41" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="B42" t="s">
         <v>690</v>
@@ -12747,16 +12791,16 @@
       <c r="D42" s="45" t="s">
         <v>691</v>
       </c>
-      <c r="E42" s="68" t="s">
+      <c r="E42" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F42" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="B43" t="s">
         <v>692</v>
@@ -12767,16 +12811,16 @@
       <c r="D43" s="45" t="s">
         <v>693</v>
       </c>
-      <c r="E43" s="68" t="s">
+      <c r="E43" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F43" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="B44" t="s">
         <v>695</v>
@@ -12787,16 +12831,16 @@
       <c r="D44" s="45" t="s">
         <v>696</v>
       </c>
-      <c r="E44" s="68" t="s">
+      <c r="E44" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F44" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="B45" t="s">
         <v>698</v>
@@ -12807,16 +12851,16 @@
       <c r="D45" s="45" t="s">
         <v>699</v>
       </c>
-      <c r="E45" s="68" t="s">
+      <c r="E45" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F45" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="B46" t="s">
         <v>701</v>
@@ -12827,16 +12871,16 @@
       <c r="D46" s="45" t="s">
         <v>702</v>
       </c>
-      <c r="E46" s="68" t="s">
+      <c r="E46" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F46" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="B47" t="s">
         <v>704</v>
@@ -12847,16 +12891,16 @@
       <c r="D47" s="45" t="s">
         <v>705</v>
       </c>
-      <c r="E47" s="68" t="s">
+      <c r="E47" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F47" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="B48" t="s">
         <v>707</v>
@@ -12867,16 +12911,16 @@
       <c r="D48" s="45" t="s">
         <v>708</v>
       </c>
-      <c r="E48" s="68" t="s">
+      <c r="E48" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F48" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="B49" t="s">
         <v>898</v>
@@ -12887,16 +12931,16 @@
       <c r="D49" s="45" t="s">
         <v>710</v>
       </c>
-      <c r="E49" s="68" t="s">
+      <c r="E49" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F49" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="B50" t="s">
         <v>711</v>
@@ -12907,16 +12951,16 @@
       <c r="D50" s="45" t="s">
         <v>712</v>
       </c>
-      <c r="E50" s="68" t="s">
+      <c r="E50" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F50" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="B51" t="s">
         <v>714</v>
@@ -12925,18 +12969,18 @@
         <v>260</v>
       </c>
       <c r="D51" s="46" t="s">
-        <v>1309</v>
-      </c>
-      <c r="E51" s="68" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E51" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F51" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="B52" t="s">
         <v>716</v>
@@ -12947,16 +12991,16 @@
       <c r="D52" s="45" t="s">
         <v>717</v>
       </c>
-      <c r="E52" s="68" t="s">
+      <c r="E52" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F52" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="B53" t="s">
         <v>718</v>
@@ -12967,16 +13011,16 @@
       <c r="D53" s="45" t="s">
         <v>719</v>
       </c>
-      <c r="E53" s="68" t="s">
+      <c r="E53" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F53" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="B54" t="s">
         <v>721</v>
@@ -12987,16 +13031,16 @@
       <c r="D54" s="45" t="s">
         <v>722</v>
       </c>
-      <c r="E54" s="68" t="s">
+      <c r="E54" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F54" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="B55" t="s">
         <v>724</v>
@@ -13007,16 +13051,16 @@
       <c r="D55" s="45" t="s">
         <v>725</v>
       </c>
-      <c r="E55" s="68" t="s">
+      <c r="E55" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F55" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="B56" t="s">
         <v>727</v>
@@ -13027,16 +13071,16 @@
       <c r="D56" s="45" t="s">
         <v>728</v>
       </c>
-      <c r="E56" s="68" t="s">
+      <c r="E56" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F56" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="B57" t="s">
         <v>730</v>
@@ -13047,16 +13091,16 @@
       <c r="D57" s="45" t="s">
         <v>731</v>
       </c>
-      <c r="E57" s="68" t="s">
+      <c r="E57" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F57" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B58" t="s">
         <v>733</v>
@@ -13067,16 +13111,16 @@
       <c r="D58" s="45" t="s">
         <v>734</v>
       </c>
-      <c r="E58" s="68" t="s">
+      <c r="E58" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F58" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="B59" t="s">
         <v>736</v>
@@ -13087,16 +13131,16 @@
       <c r="D59" s="45" t="s">
         <v>737</v>
       </c>
-      <c r="E59" s="68" t="s">
+      <c r="E59" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F59" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="B60" t="s">
         <v>739</v>
@@ -13107,16 +13151,16 @@
       <c r="D60" s="45" t="s">
         <v>740</v>
       </c>
-      <c r="E60" s="68" t="s">
+      <c r="E60" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F60" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="B61" t="s">
         <v>742</v>
@@ -13127,16 +13171,16 @@
       <c r="D61" s="45" t="s">
         <v>743</v>
       </c>
-      <c r="E61" s="68" t="s">
+      <c r="E61" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F61" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="B62" t="s">
         <v>745</v>
@@ -13147,16 +13191,16 @@
       <c r="D62" s="45" t="s">
         <v>746</v>
       </c>
-      <c r="E62" s="68" t="s">
+      <c r="E62" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F62" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="B63" t="s">
         <v>927</v>
@@ -13165,18 +13209,18 @@
         <v>260</v>
       </c>
       <c r="D63" s="46" t="s">
-        <v>1322</v>
-      </c>
-      <c r="E63" s="68" t="s">
+        <v>1320</v>
+      </c>
+      <c r="E63" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F63" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="B64" t="s">
         <v>748</v>
@@ -13187,16 +13231,16 @@
       <c r="D64" s="45" t="s">
         <v>749</v>
       </c>
-      <c r="E64" s="68" t="s">
+      <c r="E64" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F64" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="B65" t="s">
         <v>751</v>
@@ -13207,16 +13251,16 @@
       <c r="D65" s="45" t="s">
         <v>752</v>
       </c>
-      <c r="E65" s="68" t="s">
+      <c r="E65" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F65" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="B66" t="s">
         <v>754</v>
@@ -13227,16 +13271,16 @@
       <c r="D66" s="45" t="s">
         <v>755</v>
       </c>
-      <c r="E66" s="68" t="s">
+      <c r="E66" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F66" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="B67" t="s">
         <v>951</v>
@@ -13247,16 +13291,16 @@
       <c r="D67" s="45" t="s">
         <v>757</v>
       </c>
-      <c r="E67" s="68" t="s">
+      <c r="E67" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F67" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="B68" t="s">
         <v>758</v>
@@ -13267,16 +13311,16 @@
       <c r="D68" s="45" t="s">
         <v>759</v>
       </c>
-      <c r="E68" s="68" t="s">
+      <c r="E68" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F68" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="B69" t="s">
         <v>761</v>
@@ -13287,16 +13331,16 @@
       <c r="D69" s="45" t="s">
         <v>762</v>
       </c>
-      <c r="E69" s="68" t="s">
+      <c r="E69" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F69" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="B70" t="s">
         <v>763</v>
@@ -13307,16 +13351,16 @@
       <c r="D70" s="45" t="s">
         <v>764</v>
       </c>
-      <c r="E70" s="68" t="s">
+      <c r="E70" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F70" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="B71" t="s">
         <v>765</v>
@@ -13327,16 +13371,16 @@
       <c r="D71" s="45" t="s">
         <v>766</v>
       </c>
-      <c r="E71" s="68" t="s">
+      <c r="E71" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F71" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="B72" t="s">
         <v>767</v>
@@ -13347,16 +13391,16 @@
       <c r="D72" s="45" t="s">
         <v>768</v>
       </c>
-      <c r="E72" s="68" t="s">
+      <c r="E72" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F72" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="B73" t="s">
         <v>769</v>
@@ -13367,16 +13411,16 @@
       <c r="D73" s="45" t="s">
         <v>770</v>
       </c>
-      <c r="E73" s="68" t="s">
+      <c r="E73" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F73" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="B74" t="s">
         <v>771</v>
@@ -13387,16 +13431,16 @@
       <c r="D74" s="45" t="s">
         <v>772</v>
       </c>
-      <c r="E74" s="68" t="s">
+      <c r="E74" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F74" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="B75" t="s">
         <v>773</v>
@@ -13407,16 +13451,16 @@
       <c r="D75" s="45" t="s">
         <v>774</v>
       </c>
-      <c r="E75" s="68" t="s">
+      <c r="E75" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F75" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="B76" t="s">
         <v>775</v>
@@ -13427,16 +13471,16 @@
       <c r="D76" s="45" t="s">
         <v>776</v>
       </c>
-      <c r="E76" s="68" t="s">
+      <c r="E76" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F76" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="B77" t="s">
         <v>777</v>
@@ -13447,11 +13491,11 @@
       <c r="D77" s="45" t="s">
         <v>778</v>
       </c>
-      <c r="E77" s="68" t="s">
+      <c r="E77" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F77" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
     </row>
   </sheetData>
@@ -13464,16 +13508,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E75AA97-4922-F248-8DDB-BFD2366D5770}">
   <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14.33203125" style="60" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="70" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="66" customWidth="1"/>
     <col min="4" max="4" width="72" style="61" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="71" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="67" customWidth="1"/>
     <col min="6" max="6" width="14.6640625" style="60" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13484,25 +13528,25 @@
       <c r="B1" s="44" t="s">
         <v>221</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="62" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D1" s="63" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="62" t="s">
+        <v>1254</v>
+      </c>
+      <c r="F1" s="63" t="s">
         <v>1255</v>
-      </c>
-      <c r="D1" s="67" t="s">
-        <v>223</v>
-      </c>
-      <c r="E1" s="66" t="s">
-        <v>1256</v>
-      </c>
-      <c r="F1" s="67" t="s">
-        <v>1257</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1346</v>
-      </c>
-      <c r="B2" s="69" t="s">
-        <v>1259</v>
+        <v>1344</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>1257</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>500</v>
@@ -13510,16 +13554,16 @@
       <c r="D2" s="46" t="s">
         <v>590</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="64" t="s">
         <v>500</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="B3" s="47" t="s">
         <v>862</v>
@@ -13530,14 +13574,14 @@
       <c r="D3" s="46" t="s">
         <v>863</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="64" t="s">
         <v>260</v>
       </c>
       <c r="F3" s="46"/>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="B4" s="46" t="s">
         <v>864</v>
@@ -13554,7 +13598,7 @@
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="B5" s="46" t="s">
         <v>867</v>
@@ -13572,7 +13616,7 @@
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="B6" s="46" t="s">
         <v>869</v>
@@ -13587,12 +13631,12 @@
         <v>260</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="B7" s="46" t="s">
         <v>872</v>
@@ -13607,12 +13651,12 @@
         <v>260</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="B8" s="46" t="s">
         <v>875</v>
@@ -13627,12 +13671,12 @@
         <v>260</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="B9" s="46" t="s">
         <v>225</v>
@@ -13650,7 +13694,7 @@
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="B10" s="46" t="s">
         <v>878</v>
@@ -13668,7 +13712,7 @@
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="B11" s="46" t="s">
         <v>880</v>
@@ -13686,7 +13730,7 @@
     </row>
     <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="B12" s="46" t="s">
         <v>882</v>
@@ -13704,7 +13748,7 @@
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="B13" s="46" t="s">
         <v>884</v>
@@ -13722,7 +13766,7 @@
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="B14" s="46" t="s">
         <v>886</v>
@@ -13740,7 +13784,7 @@
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="B15" s="46" t="s">
         <v>888</v>
@@ -13758,7 +13802,7 @@
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="B16" s="46" t="s">
         <v>890</v>
@@ -13773,12 +13817,12 @@
         <v>260</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="B17" s="46" t="s">
         <v>892</v>
@@ -13796,7 +13840,7 @@
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="B18" s="46" t="s">
         <v>894</v>
@@ -13811,12 +13855,12 @@
         <v>260</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="B19" s="46" t="s">
         <v>896</v>
@@ -13834,7 +13878,7 @@
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="B20" s="46" t="s">
         <v>898</v>
@@ -13852,7 +13896,7 @@
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="B21" s="46" t="s">
         <v>900</v>
@@ -13867,12 +13911,12 @@
         <v>260</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="B22" s="46" t="s">
         <v>903</v>
@@ -13890,7 +13934,7 @@
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="B23" s="46" t="s">
         <v>905</v>
@@ -13908,7 +13952,7 @@
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="B24" s="46" t="s">
         <v>907</v>
@@ -13926,7 +13970,7 @@
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="B25" s="46" t="s">
         <v>909</v>
@@ -13944,7 +13988,7 @@
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="B26" s="46" t="s">
         <v>911</v>
@@ -13962,7 +14006,7 @@
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="B27" s="46" t="s">
         <v>913</v>
@@ -13980,7 +14024,7 @@
     </row>
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="B28" s="46" t="s">
         <v>915</v>
@@ -13998,7 +14042,7 @@
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="B29" s="46" t="s">
         <v>917</v>
@@ -14016,7 +14060,7 @@
     </row>
     <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="B30" s="46" t="s">
         <v>919</v>
@@ -14034,7 +14078,7 @@
     </row>
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="B31" s="46" t="s">
         <v>921</v>
@@ -14052,7 +14096,7 @@
     </row>
     <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="B32" s="46" t="s">
         <v>923</v>
@@ -14070,7 +14114,7 @@
     </row>
     <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="B33" s="46" t="s">
         <v>925</v>
@@ -14088,7 +14132,7 @@
     </row>
     <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="B34" s="46" t="s">
         <v>927</v>
@@ -14106,7 +14150,7 @@
     </row>
     <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="B35" s="46" t="s">
         <v>929</v>
@@ -14124,7 +14168,7 @@
     </row>
     <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="B36" s="46" t="s">
         <v>931</v>
@@ -14139,12 +14183,12 @@
         <v>260</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="B37" s="46" t="s">
         <v>932</v>
@@ -14159,12 +14203,12 @@
         <v>260</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="B38" s="46" t="s">
         <v>933</v>
@@ -14182,7 +14226,7 @@
     </row>
     <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="B39" s="46" t="s">
         <v>935</v>
@@ -14200,7 +14244,7 @@
     </row>
     <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="B40" s="46" t="s">
         <v>937</v>
@@ -14218,7 +14262,7 @@
     </row>
     <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="B41" s="46" t="s">
         <v>939</v>
@@ -14236,7 +14280,7 @@
     </row>
     <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="B42" s="46" t="s">
         <v>941</v>
@@ -14254,7 +14298,7 @@
     </row>
     <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="B43" s="46" t="s">
         <v>943</v>
@@ -14272,7 +14316,7 @@
     </row>
     <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="B44" s="46" t="s">
         <v>945</v>
@@ -14290,7 +14334,7 @@
     </row>
     <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="B45" s="46" t="s">
         <v>947</v>
@@ -14308,7 +14352,7 @@
     </row>
     <row r="46" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="B46" s="46" t="s">
         <v>949</v>
@@ -14326,7 +14370,7 @@
     </row>
     <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="B47" s="46" t="s">
         <v>951</v>
@@ -14344,7 +14388,7 @@
     </row>
     <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="B48" s="46" t="s">
         <v>953</v>
@@ -14362,7 +14406,7 @@
     </row>
     <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="B49" s="46" t="s">
         <v>955</v>
@@ -14380,7 +14424,7 @@
     </row>
     <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="B50" s="46" t="s">
         <v>957</v>
@@ -14398,7 +14442,7 @@
     </row>
     <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="B51" s="46" t="s">
         <v>959</v>
@@ -14416,7 +14460,7 @@
     </row>
     <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="B52" s="46" t="s">
         <v>961</v>
@@ -14434,7 +14478,7 @@
     </row>
     <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
       <c r="B53" s="46" t="s">
         <v>963</v>
@@ -14452,7 +14496,7 @@
     </row>
     <row r="54" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="B54" s="46" t="s">
         <v>965</v>
@@ -14470,7 +14514,7 @@
     </row>
     <row r="55" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="B55" s="46" t="s">
         <v>967</v>
@@ -14488,7 +14532,7 @@
     </row>
     <row r="56" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="B56" s="46" t="s">
         <v>969</v>
@@ -14506,7 +14550,7 @@
     </row>
     <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="B57" s="46" t="s">
         <v>971</v>
@@ -14524,7 +14568,7 @@
     </row>
     <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="B58" s="46" t="s">
         <v>973</v>
@@ -14542,7 +14586,7 @@
     </row>
     <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="B59" s="46" t="s">
         <v>975</v>
@@ -14560,7 +14604,7 @@
     </row>
     <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="B60" s="46" t="s">
         <v>977</v>
@@ -14578,7 +14622,7 @@
     </row>
     <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="B61" s="46" t="s">
         <v>979</v>
@@ -14596,7 +14640,7 @@
     </row>
     <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="B62" s="46" t="s">
         <v>981</v>
@@ -14614,7 +14658,7 @@
     </row>
     <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="B63" s="46" t="s">
         <v>983</v>
@@ -14632,7 +14676,7 @@
     </row>
     <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="B64" s="46" t="s">
         <v>985</v>
@@ -14650,7 +14694,7 @@
     </row>
     <row r="65" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="B65" s="46" t="s">
         <v>987</v>
@@ -14668,7 +14712,7 @@
     </row>
     <row r="66" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="B66" s="46" t="s">
         <v>989</v>
@@ -14686,7 +14730,7 @@
     </row>
     <row r="67" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="B67" s="46" t="s">
         <v>991</v>
@@ -14704,7 +14748,7 @@
     </row>
     <row r="68" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="B68" s="46" t="s">
         <v>993</v>
@@ -14722,7 +14766,7 @@
     </row>
     <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="B69" s="46" t="s">
         <v>994</v>
@@ -14740,7 +14784,7 @@
     </row>
     <row r="70" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="B70" s="46" t="s">
         <v>996</v>
@@ -14758,7 +14802,7 @@
     </row>
     <row r="71" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="B71" s="46" t="s">
         <v>998</v>
@@ -14776,7 +14820,7 @@
     </row>
     <row r="72" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="B72" s="46" t="s">
         <v>1000</v>
@@ -14794,7 +14838,7 @@
     </row>
     <row r="73" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="B73" s="46" t="s">
         <v>1002</v>
@@ -14812,7 +14856,7 @@
     </row>
     <row r="74" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="B74" s="46" t="s">
         <v>1004</v>
@@ -14830,7 +14874,7 @@
     </row>
     <row r="75" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="B75" s="46" t="s">
         <v>1006</v>
@@ -14848,7 +14892,7 @@
     </row>
     <row r="76" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="B76" s="46" t="s">
         <v>1008</v>
@@ -14866,7 +14910,7 @@
     </row>
     <row r="77" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="B77" s="46" t="s">
         <v>1010</v>
@@ -14884,7 +14928,7 @@
     </row>
     <row r="78" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="B78" s="46" t="s">
         <v>1012</v>
@@ -14902,7 +14946,7 @@
     </row>
     <row r="79" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="B79" s="46" t="s">
         <v>1014</v>
@@ -14920,7 +14964,7 @@
     </row>
     <row r="80" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="B80" s="46" t="s">
         <v>1016</v>
@@ -14938,7 +14982,7 @@
     </row>
     <row r="81" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="B81" s="46" t="s">
         <v>1018</v>
@@ -14956,7 +15000,7 @@
     </row>
     <row r="82" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="B82" s="46" t="s">
         <v>1020</v>
@@ -14974,7 +15018,7 @@
     </row>
     <row r="83" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="B83" s="46" t="s">
         <v>1022</v>
@@ -14992,7 +15036,7 @@
     </row>
     <row r="84" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
       <c r="B84" s="46" t="s">
         <v>1024</v>
@@ -15010,7 +15054,7 @@
     </row>
     <row r="85" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="B85" s="46" t="s">
         <v>1026</v>
@@ -15028,7 +15072,7 @@
     </row>
     <row r="86" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="B86" s="46" t="s">
         <v>1028</v>
@@ -15046,7 +15090,7 @@
     </row>
     <row r="87" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="B87" s="46" t="s">
         <v>1030</v>
@@ -15064,7 +15108,7 @@
     </row>
     <row r="88" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="B88" s="46" t="s">
         <v>1032</v>
@@ -15082,7 +15126,7 @@
     </row>
     <row r="89" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="B89" s="46" t="s">
         <v>1034</v>
@@ -15100,7 +15144,7 @@
     </row>
     <row r="90" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="B90" s="46" t="s">
         <v>1035</v>
@@ -15118,7 +15162,7 @@
     </row>
     <row r="91" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="B91" s="46" t="s">
         <v>1037</v>
@@ -15136,7 +15180,7 @@
     </row>
     <row r="92" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="B92" s="46" t="s">
         <v>1039</v>
@@ -15154,7 +15198,7 @@
     </row>
     <row r="93" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="B93" s="46" t="s">
         <v>1041</v>
@@ -15172,7 +15216,7 @@
     </row>
     <row r="94" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B94" s="46" t="s">
         <v>1043</v>
@@ -15190,7 +15234,7 @@
     </row>
     <row r="95" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="B95" s="46" t="s">
         <v>1045</v>
@@ -15208,7 +15252,7 @@
     </row>
     <row r="96" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="B96" s="46" t="s">
         <v>1047</v>
@@ -15226,7 +15270,7 @@
     </row>
     <row r="97" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="B97" s="46" t="s">
         <v>1049</v>
@@ -15244,7 +15288,7 @@
     </row>
     <row r="98" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="B98" s="46" t="s">
         <v>1051</v>
@@ -15262,7 +15306,7 @@
     </row>
     <row r="99" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="B99" s="46" t="s">
         <v>1053</v>
@@ -15280,7 +15324,7 @@
     </row>
     <row r="100" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="B100" s="46" t="s">
         <v>1055</v>
@@ -15298,7 +15342,7 @@
     </row>
     <row r="101" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="B101" s="46" t="s">
         <v>1057</v>
@@ -15316,7 +15360,7 @@
     </row>
     <row r="102" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="B102" s="46" t="s">
         <v>1059</v>
@@ -15334,7 +15378,7 @@
     </row>
     <row r="103" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="B103" s="46" t="s">
         <v>1061</v>
@@ -15352,7 +15396,7 @@
     </row>
     <row r="104" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="B104" s="46" t="s">
         <v>1063</v>
@@ -15370,7 +15414,7 @@
     </row>
     <row r="105" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="B105" s="46" t="s">
         <v>1065</v>
@@ -15388,7 +15432,7 @@
     </row>
     <row r="106" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="B106" s="46" t="s">
         <v>1067</v>
@@ -15406,7 +15450,7 @@
     </row>
     <row r="107" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="B107" s="46" t="s">
         <v>1069</v>
@@ -15424,7 +15468,7 @@
     </row>
     <row r="108" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="B108" s="46" t="s">
         <v>1071</v>
@@ -15442,7 +15486,7 @@
     </row>
     <row r="109" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="B109" s="46" t="s">
         <v>1073</v>
@@ -15460,7 +15504,7 @@
     </row>
     <row r="110" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="B110" s="46" t="s">
         <v>1075</v>
@@ -15478,7 +15522,7 @@
     </row>
     <row r="111" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="B111" s="46" t="s">
         <v>1077</v>
@@ -15496,7 +15540,7 @@
     </row>
     <row r="112" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="B112" s="46" t="s">
         <v>1079</v>
@@ -15514,7 +15558,7 @@
     </row>
     <row r="113" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="B113" s="46" t="s">
         <v>1081</v>
@@ -15532,7 +15576,7 @@
     </row>
     <row r="114" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="B114" s="46" t="s">
         <v>226</v>
@@ -15550,7 +15594,7 @@
     </row>
     <row r="115" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="B115" s="46" t="s">
         <v>1084</v>
@@ -15568,7 +15612,7 @@
     </row>
     <row r="116" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="B116" s="46" t="s">
         <v>1085</v>
@@ -15586,7 +15630,7 @@
     </row>
     <row r="117" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
       <c r="B117" s="46" t="s">
         <v>1087</v>
@@ -15604,7 +15648,7 @@
     </row>
     <row r="118" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="B118" s="46" t="s">
         <v>1089</v>
@@ -15622,7 +15666,7 @@
     </row>
     <row r="119" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="B119" s="46" t="s">
         <v>1091</v>
@@ -15640,7 +15684,7 @@
     </row>
     <row r="120" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="B120" s="46" t="s">
         <v>1093</v>
@@ -15658,7 +15702,7 @@
     </row>
     <row r="121" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="B121" s="46" t="s">
         <v>1095</v>
@@ -15676,7 +15720,7 @@
     </row>
     <row r="122" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="B122" s="46" t="s">
         <v>1097</v>
@@ -15694,7 +15738,7 @@
     </row>
     <row r="123" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="B123" s="46" t="s">
         <v>1099</v>
@@ -15712,7 +15756,7 @@
     </row>
     <row r="124" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="B124" s="46" t="s">
         <v>1101</v>
@@ -15730,7 +15774,7 @@
     </row>
     <row r="125" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="B125" s="46" t="s">
         <v>1103</v>
@@ -15748,7 +15792,7 @@
     </row>
     <row r="126" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="B126" s="46" t="s">
         <v>1105</v>
@@ -15766,7 +15810,7 @@
     </row>
     <row r="127" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="B127" s="46" t="s">
         <v>1107</v>
@@ -15784,7 +15828,7 @@
     </row>
     <row r="128" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="B128" s="46" t="s">
         <v>1109</v>
@@ -15802,7 +15846,7 @@
     </row>
     <row r="129" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="B129" s="46" t="s">
         <v>1111</v>
@@ -15820,7 +15864,7 @@
     </row>
     <row r="130" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="B130" s="46" t="s">
         <v>1113</v>
@@ -15838,7 +15882,7 @@
     </row>
     <row r="131" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
       <c r="B131" s="46" t="s">
         <v>1115</v>
@@ -15856,7 +15900,7 @@
     </row>
     <row r="132" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="B132" s="46" t="s">
         <v>1116</v>
@@ -15874,7 +15918,7 @@
     </row>
     <row r="133" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="B133" s="46" t="s">
         <v>1118</v>
@@ -15892,7 +15936,7 @@
     </row>
     <row r="134" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="B134" s="46" t="s">
         <v>1120</v>
@@ -15910,7 +15954,7 @@
     </row>
     <row r="135" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="B135" s="46" t="s">
         <v>1122</v>
@@ -15928,7 +15972,7 @@
     </row>
     <row r="136" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="B136" s="46" t="s">
         <v>227</v>
@@ -15946,7 +15990,7 @@
     </row>
     <row r="137" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="B137" s="46" t="s">
         <v>1125</v>
@@ -15964,7 +16008,7 @@
     </row>
     <row r="138" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="B138" s="46" t="s">
         <v>1127</v>
@@ -15982,7 +16026,7 @@
     </row>
     <row r="139" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="B139" s="46" t="s">
         <v>1129</v>
@@ -16000,7 +16044,7 @@
     </row>
     <row r="140" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="B140" s="46" t="s">
         <v>1131</v>
@@ -16018,7 +16062,7 @@
     </row>
     <row r="141" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
       <c r="B141" s="46" t="s">
         <v>1133</v>
@@ -16036,7 +16080,7 @@
     </row>
     <row r="142" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="B142" s="46" t="s">
         <v>1135</v>
@@ -16054,7 +16098,7 @@
     </row>
     <row r="143" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
       <c r="B143" s="46" t="s">
         <v>1137</v>
@@ -16072,7 +16116,7 @@
     </row>
     <row r="144" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="B144" s="46" t="s">
         <v>1139</v>
@@ -16090,7 +16134,7 @@
     </row>
     <row r="145" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
       <c r="B145" s="46" t="s">
         <v>1141</v>
@@ -16108,7 +16152,7 @@
     </row>
     <row r="146" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="B146" s="46" t="s">
         <v>1143</v>
@@ -16126,7 +16170,7 @@
     </row>
     <row r="147" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
       <c r="B147" s="46" t="s">
         <v>1145</v>
@@ -16144,7 +16188,7 @@
     </row>
     <row r="148" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="B148" s="46" t="s">
         <v>1147</v>
@@ -16162,7 +16206,7 @@
     </row>
     <row r="149" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="B149" s="46" t="s">
         <v>1149</v>
@@ -16180,7 +16224,7 @@
     </row>
     <row r="150" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="B150" s="46" t="s">
         <v>1151</v>
@@ -16198,7 +16242,7 @@
     </row>
     <row r="151" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="B151" s="46" t="s">
         <v>228</v>
@@ -16216,7 +16260,7 @@
     </row>
     <row r="152" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="B152" s="46" t="s">
         <v>1154</v>
@@ -16234,7 +16278,7 @@
     </row>
     <row r="153" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="B153" s="46" t="s">
         <v>1155</v>
@@ -16252,7 +16296,7 @@
     </row>
     <row r="154" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="B154" s="46" t="s">
         <v>1157</v>
@@ -16270,7 +16314,7 @@
     </row>
     <row r="155" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
       <c r="B155" s="46" t="s">
         <v>229</v>
@@ -16288,7 +16332,7 @@
     </row>
     <row r="156" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="B156" s="46" t="s">
         <v>230</v>
@@ -16314,14 +16358,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3AB5D9-1FE9-BF4A-BE82-FD043736B8E5}">
   <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="158" style="5" customWidth="1"/>
+    <col min="2" max="2" width="77.1640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -16334,7 +16378,7 @@
     </row>
     <row r="2" spans="1:2" ht="372" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>837</v>
@@ -16342,7 +16386,7 @@
     </row>
     <row r="3" spans="1:2" ht="323" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="B3" s="46" t="s">
         <v>836</v>
@@ -16350,13 +16394,13 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="B4" s="13"/>
     </row>
     <row r="5" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="B5" s="46" t="s">
         <v>834</v>
@@ -16364,7 +16408,7 @@
     </row>
     <row r="6" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="B6" s="46" t="s">
         <v>835</v>
@@ -16372,13 +16416,13 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="B7" s="13"/>
     </row>
-    <row r="8" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="B8" s="46" t="s">
         <v>599</v>
@@ -16386,7 +16430,7 @@
     </row>
     <row r="9" spans="1:2" ht="136" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="B9" s="46" t="s">
         <v>602</v>
@@ -16394,7 +16438,7 @@
     </row>
     <row r="10" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="B10" s="46" t="s">
         <v>605</v>
@@ -16402,7 +16446,7 @@
     </row>
     <row r="11" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="B11" s="46" t="s">
         <v>608</v>
@@ -16410,13 +16454,13 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="B12" s="13"/>
     </row>
     <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="B13" s="46" t="s">
         <v>613</v>
@@ -16424,7 +16468,7 @@
     </row>
     <row r="14" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="B14" s="46" t="s">
         <v>838</v>
@@ -16432,7 +16476,7 @@
     </row>
     <row r="15" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="B15" s="46" t="s">
         <v>618</v>
@@ -16440,7 +16484,7 @@
     </row>
     <row r="16" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="B16" s="46" t="s">
         <v>779</v>
@@ -16448,7 +16492,7 @@
     </row>
     <row r="17" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="B17" s="46" t="s">
         <v>623</v>
@@ -16456,7 +16500,7 @@
     </row>
     <row r="18" spans="1:2" ht="170" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="B18" s="46" t="s">
         <v>626</v>
@@ -16464,7 +16508,7 @@
     </row>
     <row r="19" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="B19" s="46" t="s">
         <v>629</v>
@@ -16472,7 +16516,7 @@
     </row>
     <row r="20" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="B20" s="46" t="s">
         <v>632</v>
@@ -16480,21 +16524,21 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="B21" s="13"/>
     </row>
     <row r="22" spans="1:2" ht="187" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="B22" s="46" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="B23" s="46" t="s">
         <v>640</v>
@@ -16502,7 +16546,7 @@
     </row>
     <row r="24" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="B24" s="46" t="s">
         <v>643</v>
@@ -16510,7 +16554,7 @@
     </row>
     <row r="25" spans="1:2" ht="238" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="B25" s="46" t="s">
         <v>646</v>
@@ -16518,13 +16562,13 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="B26" s="13"/>
     </row>
     <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="B27" s="46" t="s">
         <v>651</v>
@@ -16532,7 +16576,7 @@
     </row>
     <row r="28" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="B28" s="46" t="s">
         <v>855</v>
@@ -16540,7 +16584,7 @@
     </row>
     <row r="29" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="B29" s="46" t="s">
         <v>656</v>
@@ -16548,7 +16592,7 @@
     </row>
     <row r="30" spans="1:2" ht="187" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="B30" s="46" t="s">
         <v>659</v>
@@ -16556,7 +16600,7 @@
     </row>
     <row r="31" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="B31" s="46" t="s">
         <v>661</v>
@@ -16564,7 +16608,7 @@
     </row>
     <row r="32" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="B32" s="46" t="s">
         <v>664</v>
@@ -16572,7 +16616,7 @@
     </row>
     <row r="33" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="B33" s="46" t="s">
         <v>667</v>
@@ -16580,7 +16624,7 @@
     </row>
     <row r="34" spans="1:2" ht="170" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="B34" s="46" t="s">
         <v>670</v>
@@ -16588,23 +16632,23 @@
     </row>
     <row r="35" spans="1:2" ht="238" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="B35" s="46" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="B36" s="48" t="s">
         <v>839</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="B37" s="46" t="s">
         <v>840</v>
@@ -16612,7 +16656,7 @@
     </row>
     <row r="38" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="B38" s="46" t="s">
         <v>680</v>
@@ -16620,7 +16664,7 @@
     </row>
     <row r="39" spans="1:2" ht="204" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="B39" s="46" t="s">
         <v>683</v>
@@ -16628,7 +16672,7 @@
     </row>
     <row r="40" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="B40" s="46" t="s">
         <v>686</v>
@@ -16636,7 +16680,7 @@
     </row>
     <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="B41" s="46" t="s">
         <v>689</v>
@@ -16644,13 +16688,13 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="B42" s="13"/>
     </row>
     <row r="43" spans="1:2" ht="238" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="B43" s="46" t="s">
         <v>694</v>
@@ -16658,7 +16702,7 @@
     </row>
     <row r="44" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="B44" s="46" t="s">
         <v>697</v>
@@ -16666,7 +16710,7 @@
     </row>
     <row r="45" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="B45" s="46" t="s">
         <v>700</v>
@@ -16674,7 +16718,7 @@
     </row>
     <row r="46" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="B46" s="46" t="s">
         <v>703</v>
@@ -16682,7 +16726,7 @@
     </row>
     <row r="47" spans="1:2" ht="289" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="B47" s="46" t="s">
         <v>706</v>
@@ -16690,7 +16734,7 @@
     </row>
     <row r="48" spans="1:2" ht="306" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="B48" s="46" t="s">
         <v>709</v>
@@ -16698,13 +16742,13 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="B49" s="13"/>
     </row>
     <row r="50" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="B50" s="46" t="s">
         <v>713</v>
@@ -16712,7 +16756,7 @@
     </row>
     <row r="51" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="B51" s="46" t="s">
         <v>715</v>
@@ -16720,13 +16764,13 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="B52" s="13"/>
     </row>
     <row r="53" spans="1:2" ht="323" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="B53" s="46" t="s">
         <v>720</v>
@@ -16734,7 +16778,7 @@
     </row>
     <row r="54" spans="1:2" ht="238" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="B54" s="46" t="s">
         <v>723</v>
@@ -16742,7 +16786,7 @@
     </row>
     <row r="55" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="B55" s="46" t="s">
         <v>726</v>
@@ -16750,7 +16794,7 @@
     </row>
     <row r="56" spans="1:2" ht="272" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="B56" s="46" t="s">
         <v>729</v>
@@ -16758,7 +16802,7 @@
     </row>
     <row r="57" spans="1:2" ht="306" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="B57" s="46" t="s">
         <v>732</v>
@@ -16766,7 +16810,7 @@
     </row>
     <row r="58" spans="1:2" ht="204" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="B58" s="46" t="s">
         <v>735</v>
@@ -16774,7 +16818,7 @@
     </row>
     <row r="59" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A59" s="11" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="B59" s="46" t="s">
         <v>738</v>
@@ -16782,7 +16826,7 @@
     </row>
     <row r="60" spans="1:2" ht="170" x14ac:dyDescent="0.2">
       <c r="A60" s="11" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="B60" s="46" t="s">
         <v>741</v>
@@ -16790,7 +16834,7 @@
     </row>
     <row r="61" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="B61" s="46" t="s">
         <v>744</v>
@@ -16798,7 +16842,7 @@
     </row>
     <row r="62" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A62" s="11" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="B62" s="46" t="s">
         <v>747</v>
@@ -16806,13 +16850,13 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="B63" s="13"/>
     </row>
     <row r="64" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="B64" s="46" t="s">
         <v>750</v>
@@ -16820,7 +16864,7 @@
     </row>
     <row r="65" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="B65" s="46" t="s">
         <v>753</v>
@@ -16828,15 +16872,15 @@
     </row>
     <row r="66" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="B66" s="46" t="s">
         <v>756</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="B67" s="46" t="s">
         <v>780</v>
@@ -16844,7 +16888,7 @@
     </row>
     <row r="68" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="B68" s="46" t="s">
         <v>841</v>
@@ -16852,7 +16896,7 @@
     </row>
     <row r="69" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="11" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="B69" s="46" t="s">
         <v>760</v>
@@ -16860,7 +16904,7 @@
     </row>
     <row r="70" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="B70" s="46" t="s">
         <v>760</v>
@@ -16868,7 +16912,7 @@
     </row>
     <row r="71" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="11" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="B71" s="46" t="s">
         <v>760</v>
@@ -16876,7 +16920,7 @@
     </row>
     <row r="72" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="11" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="B72" s="46" t="s">
         <v>760</v>
@@ -16884,7 +16928,7 @@
     </row>
     <row r="73" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="11" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="B73" s="46" t="s">
         <v>760</v>
@@ -16892,7 +16936,7 @@
     </row>
     <row r="74" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="11" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="B74" s="46" t="s">
         <v>760</v>
@@ -16900,7 +16944,7 @@
     </row>
     <row r="75" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="11" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="B75" s="46" t="s">
         <v>760</v>
@@ -16908,7 +16952,7 @@
     </row>
     <row r="76" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="11" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="B76" s="46" t="s">
         <v>760</v>
@@ -16916,7 +16960,7 @@
     </row>
     <row r="77" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="11" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="B77" s="46" t="s">
         <v>760</v>
@@ -16924,7 +16968,7 @@
     </row>
     <row r="78" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="11" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="B78" s="46" t="s">
         <v>866</v>
@@ -16932,7 +16976,7 @@
     </row>
     <row r="79" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="B79" s="46" t="s">
         <v>871</v>
@@ -16940,7 +16984,7 @@
     </row>
     <row r="80" spans="1:2" ht="356" x14ac:dyDescent="0.2">
       <c r="A80" s="11" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="B80" s="46" t="s">
         <v>874</v>
@@ -16948,7 +16992,7 @@
     </row>
     <row r="81" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="11" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="B81" s="46" t="s">
         <v>841</v>
@@ -16956,7 +17000,7 @@
     </row>
     <row r="82" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A82" s="11" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="B82" s="46" t="s">
         <v>834</v>
@@ -16964,7 +17008,7 @@
     </row>
     <row r="83" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A83" s="11" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="B83" s="46" t="s">
         <v>835</v>
@@ -16972,7 +17016,7 @@
     </row>
     <row r="84" spans="1:2" ht="204" x14ac:dyDescent="0.2">
       <c r="A84" s="11" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="B84" s="46" t="s">
         <v>902</v>
@@ -16980,7 +17024,7 @@
     </row>
     <row r="85" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="11" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="B85" s="46" t="s">
         <v>618</v>
@@ -16988,7 +17032,7 @@
     </row>
     <row r="86" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A86" s="11" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="B86" s="46" t="s">
         <v>779</v>
@@ -17002,15 +17046,16 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED6534B-B4C9-924A-BB14-180C2C37C6F1}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17064,15 +17109,7 @@
         <v>1162</v>
       </c>
       <c r="B6" t="s">
-        <v>1164</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
         <v>1163</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1178</v>
       </c>
     </row>
   </sheetData>
@@ -17184,144 +17221,144 @@
       <c r="A1" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="68" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="69" t="s">
         <v>534</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
     </row>
     <row r="4" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="68" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="68" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="70" t="s">
         <v>419</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
       <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>525</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="68" t="s">
         <v>526</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>527</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="68" t="s">
         <v>528</v>
       </c>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="68" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="62" t="s">
+      <c r="B12" s="71" t="s">
         <v>437</v>
       </c>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
-      <c r="E12" s="62"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -17413,11 +17450,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B4:F4"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
@@ -17425,6 +17457,11 @@
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17651,7 +17688,7 @@
         <v>801</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -17770,7 +17807,7 @@
         <v>828</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -17804,7 +17841,7 @@
         <v>807</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -17838,7 +17875,7 @@
         <v>809</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="153" x14ac:dyDescent="0.2">
@@ -17855,7 +17892,7 @@
         <v>810</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="153" x14ac:dyDescent="0.2">
@@ -17872,7 +17909,7 @@
         <v>811</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="136" x14ac:dyDescent="0.2">
@@ -17889,7 +17926,7 @@
         <v>812</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -17906,7 +17943,7 @@
         <v>829</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -17923,7 +17960,7 @@
         <v>813</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -17940,7 +17977,7 @@
         <v>814</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -17974,7 +18011,7 @@
         <v>816</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -18042,7 +18079,7 @@
         <v>821</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -18093,7 +18130,7 @@
         <v>824</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
   </sheetData>
@@ -20864,6 +20901,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -21064,15 +21110,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -21085,6 +21122,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21099,14 +21144,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add roles to CDISC Pilot Study
</commit_message>
<xml_diff>
--- a/source_data/protocols/CDISC_Pilot/CDISC_Pilot_Study.xlsx
+++ b/source_data/protocols/CDISC_Pilot/CDISC_Pilot_Study.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/protocols/CDISC_Pilot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EC08D8-C97F-CA4C-BEC5-205632454D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FB971A-267E-7A47-AD49-06817E2B94E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28440" yWindow="500" windowWidth="41180" windowHeight="27240" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="23760" yWindow="500" windowWidth="41180" windowHeight="27240" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -38,10 +38,11 @@
     <sheet name="studyDesignEncounters" sheetId="12" r:id="rId23"/>
     <sheet name="studyDesignElements" sheetId="13" r:id="rId24"/>
     <sheet name="dictionaries" sheetId="20" r:id="rId25"/>
-    <sheet name="lillyFormat" sheetId="16" r:id="rId26"/>
-    <sheet name="m11Format" sheetId="28" r:id="rId27"/>
-    <sheet name="documentContent" sheetId="29" r:id="rId28"/>
-    <sheet name="configuration" sheetId="10" r:id="rId29"/>
+    <sheet name="roles" sheetId="31" r:id="rId26"/>
+    <sheet name="lillyFormat" sheetId="16" r:id="rId27"/>
+    <sheet name="m11Format" sheetId="28" r:id="rId28"/>
+    <sheet name="documentContent" sheetId="29" r:id="rId29"/>
+    <sheet name="configuration" sheetId="10" r:id="rId30"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3177" uniqueCount="1503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3190" uniqueCount="1510">
   <si>
     <t>Screening</t>
   </si>
@@ -6698,6 +6699,27 @@
   <si>
     <t>Clinical Development Plan</t>
   </si>
+  <si>
+    <t>people</t>
+  </si>
+  <si>
+    <t>organizations</t>
+  </si>
+  <si>
+    <t>ROLE_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masked </t>
+  </si>
+  <si>
+    <t>Sponsor role</t>
+  </si>
+  <si>
+    <t>Sponsor</t>
+  </si>
+  <si>
+    <t>sponsor</t>
+  </si>
 </sst>
 </file>
 
@@ -7034,19 +7056,19 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -14510,6 +14532,68 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666D5CD6-DF98-6447-9150-7AA4E8F8C9F3}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>1503</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>525</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>463</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1505</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1508</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1506</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1509</v>
+      </c>
+      <c r="G2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:F77"/>
   <sheetViews>
@@ -16072,7 +16156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E75AA97-4922-F248-8DDB-BFD2366D5770}">
   <dimension ref="A1:F156"/>
   <sheetViews>
@@ -18922,7 +19006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3AB5D9-1FE9-BF4A-BE82-FD043736B8E5}">
   <dimension ref="A1:B86"/>
   <sheetViews>
@@ -19618,7 +19702,90 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A054F5-5F55-D04A-9603-B97FC15141C8}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="66.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E3" t="s">
+        <v>267</v>
+      </c>
+      <c r="F3" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED6534B-B4C9-924A-BB14-180C2C37C6F1}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -19686,94 +19853,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A054F5-5F55-D04A-9603-B97FC15141C8}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="5" width="30.6640625" customWidth="1"/>
-    <col min="6" max="6" width="66.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="C2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F2" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>263</v>
-      </c>
-      <c r="B3" t="s">
-        <v>264</v>
-      </c>
-      <c r="C3" t="s">
-        <v>265</v>
-      </c>
-      <c r="D3" t="s">
-        <v>266</v>
-      </c>
-      <c r="E3" t="s">
-        <v>267</v>
-      </c>
-      <c r="F3" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEE339AA-95CC-C648-B549-41E87315C022}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -19789,28 +19873,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="68" t="s">
         <v>239</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="F1" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="72" t="s">
+      <c r="G1" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="72" t="s">
+      <c r="H1" s="68" t="s">
         <v>1499</v>
       </c>
     </row>
@@ -19893,25 +19977,25 @@
       <c r="A3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="70" t="s">
         <v>534</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
     </row>
     <row r="4" spans="1:6" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="71" t="s">
         <v>123</v>
       </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
@@ -19941,7 +20025,7 @@
       <c r="A7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="71" t="s">
         <v>419</v>
       </c>
       <c r="C7" s="69"/>
@@ -20001,12 +20085,12 @@
       <c r="A12" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="72" t="s">
         <v>437</v>
       </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="68"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -20098,11 +20182,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B4:F4"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B5:E5"/>
@@ -20110,6 +20189,11 @@
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20995,6 +21079,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -21195,27 +21299,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21232,29 +21341,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>